<commit_message>
Updated BOM file ( October 25,2017 )
</commit_message>
<xml_diff>
--- a/LipSync_BOM.xlsx
+++ b/LipSync_BOM.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Milad\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Milad\Development\makersmakingchange\LipSync\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22812" windowHeight="8520"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LipSync_BOM" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="230">
   <si>
     <t>Qty</t>
   </si>
@@ -36,9 +36,6 @@
     <t>SKU</t>
   </si>
   <si>
-    <t>URL</t>
-  </si>
-  <si>
     <t>Digi-Key</t>
   </si>
   <si>
@@ -63,18 +60,12 @@
     <t>Amazon</t>
   </si>
   <si>
-    <t xml:space="preserve">Arduino Micro / Genuino Micro </t>
-  </si>
-  <si>
     <t>A000053</t>
   </si>
   <si>
     <t>Arduino</t>
   </si>
   <si>
-    <t>1050-1066-ND</t>
-  </si>
-  <si>
     <t>https://www.digikey.ca/product-detail/en/arduino/A000053/1050-1066-ND</t>
   </si>
   <si>
@@ -105,9 +96,6 @@
     <t>MPXV7002DPT1CT-ND</t>
   </si>
   <si>
-    <t>http://www.digikey.ca/product-detail/en/nxp-usa-inc/MPXV7002DPT1/MPXV7002DPT1CT-ND</t>
-  </si>
-  <si>
     <t xml:space="preserve">Right Angle Push Button </t>
   </si>
   <si>
@@ -147,15 +135,6 @@
     <t xml:space="preserve"> 0.01 uF Ceramic Through-Hole Radial Capacitor  </t>
   </si>
   <si>
-    <t xml:space="preserve">C315C103K5R5TA7303 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">399-9858-1-ND </t>
-  </si>
-  <si>
-    <t>80-C315C103K5R-TR</t>
-  </si>
-  <si>
     <t>http://www.digikey.ca/product-detail/en/kemet/C315C103K5R5TA7303/399-9858-1-ND</t>
   </si>
   <si>
@@ -216,18 +195,6 @@
     <t>http://www.digikey.ca/product-detail/en/sullins-connector-solutions/PPPC041LFBN-RC/S7037-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">3-Position Right Angle Female Through-Hole Header </t>
-  </si>
-  <si>
-    <t>PPPC031LGBN-RC</t>
-  </si>
-  <si>
-    <t>S5478-ND</t>
-  </si>
-  <si>
-    <t>http://www.digikey.ca/product-detail/en/sullins-connector-solutions/PPPC031LGBN-RC/S5478-ND</t>
-  </si>
-  <si>
     <t xml:space="preserve">17-Position Straight Female Through-Hole Headers </t>
   </si>
   <si>
@@ -255,15 +222,6 @@
     <t xml:space="preserve">Jumper Shunt Connector </t>
   </si>
   <si>
-    <t>SPC02SYAN</t>
-  </si>
-  <si>
-    <t>S9001-ND</t>
-  </si>
-  <si>
-    <t>http://www.digikey.ca/product-detail/en/sullins-connector-solutions/SPC02SYAN/S9001-ND</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sip and Puff Mouthpiece </t>
   </si>
   <si>
@@ -276,9 +234,6 @@
     <t xml:space="preserve">Filter PTFE Hydrophobic 17 mm, 0.2 Micron </t>
   </si>
   <si>
-    <t>"28213 "</t>
-  </si>
-  <si>
     <t>"28213"</t>
   </si>
   <si>
@@ -309,24 +264,6 @@
     <t>http://www.digikey.com/product-detail/en/interlink-electronics/30-49649/1027-1000-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">Screw M3 </t>
-  </si>
-  <si>
-    <t>"29341"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Keystone </t>
-  </si>
-  <si>
-    <t xml:space="preserve">36-29341-ND </t>
-  </si>
-  <si>
-    <t xml:space="preserve">534-29341 </t>
-  </si>
-  <si>
-    <t>http://www.digikey.com/product-detail/en/keystone-electronics/29341/36-29341-ND</t>
-  </si>
-  <si>
     <t xml:space="preserve">Compression Spring  </t>
   </si>
   <si>
@@ -381,15 +318,6 @@
     <t xml:space="preserve">Bumper </t>
   </si>
   <si>
-    <t>SJ-5003 (GRAY)</t>
-  </si>
-  <si>
-    <t>SJ5003-8-ND</t>
-  </si>
-  <si>
-    <t>http://www.digikey.com/product-detail/en/3m/SJ-5003-(BLACK)/SJ5003-0-ND/</t>
-  </si>
-  <si>
     <t xml:space="preserve">Nut M3 </t>
   </si>
   <si>
@@ -402,9 +330,6 @@
     <t>H762-ND</t>
   </si>
   <si>
-    <t>http://www.digikey.com/product-detail/en/b-f-fastener-supply/MHNZ-003/H762-ND/</t>
-  </si>
-  <si>
     <t xml:space="preserve">Tubing Tygon 3350 3/32" ID x 45mm </t>
   </si>
   <si>
@@ -456,9 +381,6 @@
     <t>Startech</t>
   </si>
   <si>
-    <t>https://www.amazon.com/StarTech-com-Micro-USB-Cable-UUSBHAUB3RA/dp/B001AR4NC8/ref=sr_1_1?ie=UTF8&amp;qid=1487192451&amp;sr=8-1</t>
-  </si>
-  <si>
     <t xml:space="preserve">USB Splitter </t>
   </si>
   <si>
@@ -468,24 +390,9 @@
     <t xml:space="preserve"> USB Splitter  </t>
   </si>
   <si>
-    <t>https://www.amazon.com/Micro-Female-Cable-Power-Splitter/dp/B00NSBVNCM/ref=sr_1_1?ie=UTF8&amp;qid=1488094439&amp;sr=8-1</t>
-  </si>
-  <si>
     <t xml:space="preserve">Cable Tie </t>
   </si>
   <si>
-    <t>PLT.6SM-C</t>
-  </si>
-  <si>
-    <t>Panduit</t>
-  </si>
-  <si>
-    <t>298-1016-ND</t>
-  </si>
-  <si>
-    <t>http://www.digikey.com/product-detail/en/panduit-corp/PLT.6SM-C/298-1016-ND/</t>
-  </si>
-  <si>
     <t xml:space="preserve">Magic Arm 11" and Clamp </t>
   </si>
   <si>
@@ -495,9 +402,6 @@
     <t xml:space="preserve">YKS / GkGk </t>
   </si>
   <si>
-    <t>https://www.amazon.com/GkGk-Articulating-Friction-Adjustable-Monitor/dp/B017HKJVL4/ref=sr_1_2?ie=UTF8&amp;qid=1488094690&amp;sr=8-2-spons</t>
-  </si>
-  <si>
     <t xml:space="preserve">Threaded Adapter 5/8"-27 </t>
   </si>
   <si>
@@ -507,9 +411,6 @@
     <t xml:space="preserve">CAMVATE </t>
   </si>
   <si>
-    <t>https://www.amazon.com/CAMVATE-Female-Male-Piece-Adapter/dp/B01GWVQ022/ref=sr_1_1?ie=UTF8&amp;qid=1488095005&amp;sr=8-1</t>
-  </si>
-  <si>
     <t xml:space="preserve">Velcro Cable Tie </t>
   </si>
   <si>
@@ -549,24 +450,12 @@
     <t>https://www.digikey.ca/product-detail/en/sullins-connector-solutions/PPPC061LFBN-RC/S7039-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">Cable Ties </t>
-  </si>
-  <si>
-    <t>http://www.digikey.ca/product-detail/en/te-connectivity-raychem-cable-protection/2-604771-9/2-604771-9-ND</t>
-  </si>
-  <si>
     <t xml:space="preserve">2-604771-9 </t>
   </si>
   <si>
-    <t xml:space="preserve">TE Connectivity Raychem Cable Protection </t>
-  </si>
-  <si>
     <t xml:space="preserve">2-604771-9-ND </t>
   </si>
   <si>
-    <t>571-2-604771-9</t>
-  </si>
-  <si>
     <t>10k Ohm 1/4W Mini Axial Through-Hole Resistor</t>
   </si>
   <si>
@@ -579,28 +468,253 @@
     <t>https://www.digikey.ca/product-detail/en/stackpole-electronics-inc/CFM14JT10K0/S10KQCT-ND/</t>
   </si>
   <si>
-    <t>3mm Bi-Color Through-Hole LED</t>
-  </si>
-  <si>
-    <t>SSL-LX3059IGW</t>
-  </si>
-  <si>
-    <t>Lumex</t>
-  </si>
-  <si>
-    <t>67-1327-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ca/product-detail/en/lumex-opto-components-inc/SSL-LX3059IGW/67-1327-ND/</t>
-  </si>
-  <si>
-    <t>Component name (March 21,2017)</t>
+    <t>Arduino Micro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1050-1066-ND </t>
+  </si>
+  <si>
+    <t xml:space="preserve">399-4148-ND </t>
+  </si>
+  <si>
+    <t xml:space="preserve">C315C103K5R5TA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1212-1180-ND </t>
+  </si>
+  <si>
+    <t xml:space="preserve">801-87-003-10-001101 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-Position Right Angle Male Through-Hole Header </t>
+  </si>
+  <si>
+    <t xml:space="preserve">WM4101-ND </t>
+  </si>
+  <si>
+    <t xml:space="preserve">22-05-2031 </t>
+  </si>
+  <si>
+    <t>Molex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-Position Straight Female Through-Hole Header </t>
+  </si>
+  <si>
+    <t>Preci-Dip</t>
+  </si>
+  <si>
+    <t>5mm Bi-Color Through-Hole LED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MV5437 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1080-1109-ND </t>
+  </si>
+  <si>
+    <t xml:space="preserve">S9002-ND </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSC02SYAN </t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/sullins-connector-solutions/SPC02SYAN/S9002-ND</t>
+  </si>
+  <si>
+    <t>Screws Phillips Head M3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RP809-ND </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NMS-308 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Essentra Components </t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/essentra-components/NMS-308/RP809-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SJ5003-0-ND </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SJ-5003 (BLACK) </t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/3m/SJ-5003-(BLACK)/SJ5003-0-ND/102573</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/te-connectivity-raychem-cable-protection/2-604771-9/2-604771-9-ND/2259327</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TE Connectivity Raychem </t>
+  </si>
+  <si>
+    <t>Component name (October 25,2017)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Component </t>
+  </si>
+  <si>
+    <t>Optional</t>
+  </si>
+  <si>
+    <t>Required</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/b-f-fastener-supply/MHNZ-003/H762-ND/274973</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/molex-connector-corporation/22-05-2031/WM4101-ND/</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/preci-dip/801-87-003-10-001101/1212-1180-ND</t>
+  </si>
+  <si>
+    <t>Everlight Electronics Co Ltd</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/everlight-electronics-co-ltd/MV5437/1080-1109-ND/2675600</t>
+  </si>
+  <si>
+    <t>URL ( Canada )</t>
+  </si>
+  <si>
+    <t>URL ( United States )</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/arduino/A000053/1050-1066-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/wurth-electronics-inc/431256058736/431256058736-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/stackpole-electronics-inc/CF14JT300R/CF14JT300RCT-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/stackpole-electronics-inc/CFM14JT10K0/S10KQCT-ND/</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/molex-connector-corporation/22-05-2031/WM4101-ND/</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/preci-dip/801-87-003-10-001101/1212-1180-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/sullins-connector-solutions/PPPC041LFBN-RC/S7037-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/sullins-connector-solutions/SPC02SYAN/S9002-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/sullins-connector-solutions/PPPC061LFBN-RC/S7039-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/essentra-components/NMS-308/RP809-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/te-connectivity-raychem-cable-protection/2-604771-9/2-604771-9-ND/2259327</t>
+  </si>
+  <si>
+    <t>http://www.digikey.ca/product-detail/en/interlink-electronics/30-49649/1027-1000-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.ca/product-detail/en/keystone-electronics/25501/36-25501-ND/</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/StarTech-com-Micro-USB-Cable-UUSBHAUB3RA/dp/B001AR4NC8</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Micro-Female-Cable-Power-Splitter/dp/B00NSBVNCM</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/GkGk-Articulating-Friction-Adjustable-Monitor/dp/B017HKJVL4/</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/kemet/C315C103K5R5TA7303/399-9858-1-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/kemet/C315C105K3R5TA/399-9714-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/kemet/C315C471K5R5TA/399-9740-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/sullins-connector-solutions/PPPC171LFBN-RC/S7050-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/sullins-connector-solutions/PRPC040SAAN-RC/S1011EC-40-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/everlight-electronics-co-ltd/MV5437/1080-1109-ND/2675601</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/fairchild-on-semiconductor/2N3906TFR/2N3906D26ZCT-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/3m/929974-01-01/929974-01-01-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/keystone-electronics/25503/36-25503-ND/</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/3m/SJ-5003-(BLACK)/SJ5003-0-ND/102574</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/b-f-fastener-supply/MHNZ-003/H762-ND/274974</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/sparkfun-electronics/WRL-12576/1568-1265-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/freescale-semiconductor-nxp/MPXV7002DPT1/MPXV7002DPT1CT-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/freescale-semiconductor-nxp/MPXV7002DPT1/MPXV7002DPT1CT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">571-2-604771-9 </t>
+  </si>
+  <si>
+    <t>80-C315C103K5R</t>
+  </si>
+  <si>
+    <t>841-MPXV7002DP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">782-A000053 </t>
+  </si>
+  <si>
+    <t>80-C315C105K3R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80-C315C471K5R </t>
+  </si>
+  <si>
+    <t>534-25501</t>
+  </si>
+  <si>
+    <t>534-25503</t>
+  </si>
+  <si>
+    <t>517-SJ-5003BK</t>
+  </si>
+  <si>
+    <t>645-515-1303-0250F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C315C471K5R5TA </t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/CAMVATE-Female-Male-Piece-Adapter/dp/B01GWVQ022</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1087,9 +1201,11 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1445,38 +1561,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N41"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:P41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="50.5546875" customWidth="1"/>
-    <col min="3" max="3" width="21.77734375" customWidth="1"/>
-    <col min="5" max="5" width="21" customWidth="1"/>
+    <col min="3" max="3" width="50.5546875" customWidth="1"/>
+    <col min="4" max="4" width="35.44140625" customWidth="1"/>
+    <col min="6" max="6" width="24.88671875" customWidth="1"/>
+    <col min="7" max="7" width="27.6640625" customWidth="1"/>
+    <col min="8" max="8" width="13.21875" customWidth="1"/>
+    <col min="15" max="15" width="18.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
       <c r="C1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
       </c>
       <c r="G1" t="s">
         <v>4</v>
@@ -1500,1009 +1619,1282 @@
         <v>4</v>
       </c>
       <c r="N1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O1" t="s">
+        <v>186</v>
+      </c>
+      <c r="P1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="G2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>6</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>7</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>8</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>9</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>10</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>11</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
         <v>12</v>
       </c>
-      <c r="M2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>180</v>
+      </c>
+      <c r="C3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" t="s">
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>150</v>
+      </c>
+      <c r="H3" t="s">
+        <v>221</v>
+      </c>
+      <c r="O3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P3" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>180</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" t="s">
+        <v>28</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" t="s">
+        <v>136</v>
+      </c>
+      <c r="E5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" t="s">
+        <v>136</v>
+      </c>
+      <c r="G5" t="s">
+        <v>137</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>180</v>
+      </c>
+      <c r="C6" t="s">
+        <v>145</v>
+      </c>
+      <c r="D6" t="s">
+        <v>146</v>
+      </c>
+      <c r="E6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" t="s">
+        <v>146</v>
+      </c>
+      <c r="G6" t="s">
+        <v>147</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A7">
         <v>1</v>
       </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="B7" t="s">
+        <v>180</v>
+      </c>
+      <c r="C7" t="s">
         <v>21</v>
       </c>
-      <c r="E4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="D7" t="s">
         <v>22</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="E7" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="F7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" t="s">
+        <v>220</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
         <v>1</v>
       </c>
-      <c r="B5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G5" t="s">
-        <v>25</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>2</v>
-      </c>
-      <c r="B6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" t="s">
-        <v>32</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>2</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="B8" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C7" t="s">
-        <v>169</v>
-      </c>
-      <c r="D7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" t="s">
-        <v>169</v>
-      </c>
-      <c r="F7" t="s">
-        <v>170</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>4</v>
-      </c>
-      <c r="B8" t="s">
-        <v>182</v>
-      </c>
-      <c r="C8" t="s">
-        <v>183</v>
-      </c>
-      <c r="D8" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8" t="s">
-        <v>183</v>
-      </c>
-      <c r="F8" t="s">
-        <v>184</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="F8" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="P8" s="3" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>180</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D9" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G9" t="s">
-        <v>37</v>
-      </c>
-      <c r="N9" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+      <c r="H9" t="s">
+        <v>222</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>180</v>
       </c>
       <c r="C10" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="D10" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E10" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="F10" t="s">
-        <v>43</v>
+        <v>228</v>
       </c>
       <c r="G10" t="s">
-        <v>44</v>
-      </c>
-      <c r="N10" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+      <c r="H10" t="s">
+        <v>223</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>46</v>
+        <v>180</v>
       </c>
       <c r="C11" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="D11" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="E11" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="F11" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="G11" t="s">
-        <v>47</v>
-      </c>
-      <c r="N11" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>1</v>
-      </c>
-      <c r="B12" t="s">
-        <v>50</v>
-      </c>
-      <c r="C12" t="s">
-        <v>51</v>
-      </c>
-      <c r="D12" t="s">
-        <v>52</v>
-      </c>
-      <c r="E12" t="s">
-        <v>51</v>
-      </c>
-      <c r="F12" t="s">
-        <v>53</v>
-      </c>
-      <c r="G12" t="s">
-        <v>51</v>
-      </c>
-      <c r="N12" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>1</v>
-      </c>
-      <c r="B13" t="s">
-        <v>55</v>
-      </c>
-      <c r="C13" t="s">
-        <v>56</v>
-      </c>
-      <c r="D13" t="s">
-        <v>57</v>
-      </c>
-      <c r="E13" t="s">
-        <v>56</v>
-      </c>
-      <c r="F13" t="s">
-        <v>58</v>
-      </c>
-      <c r="N13" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>2</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="P12" s="3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>2</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="O13" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="P13" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>60</v>
+        <v>180</v>
       </c>
       <c r="C14" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="D14" t="s">
+        <v>54</v>
+      </c>
+      <c r="E14" t="s">
+        <v>55</v>
+      </c>
+      <c r="F14" t="s">
+        <v>54</v>
+      </c>
+      <c r="G14" t="s">
+        <v>56</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>180</v>
+      </c>
+      <c r="C15" t="s">
         <v>62</v>
       </c>
-      <c r="E14" t="s">
-        <v>61</v>
-      </c>
-      <c r="F14" t="s">
+      <c r="D15" t="s">
         <v>63</v>
       </c>
-      <c r="N14" s="1" t="s">
+      <c r="E15" t="s">
+        <v>55</v>
+      </c>
+      <c r="F15" t="s">
+        <v>63</v>
+      </c>
+      <c r="G15" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>2</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="O15" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C15" t="s">
+      <c r="P15" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>1</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="O16" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="P16" s="3" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>1</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D15" t="s">
-        <v>62</v>
-      </c>
-      <c r="E15" t="s">
-        <v>66</v>
-      </c>
-      <c r="F15" t="s">
-        <v>67</v>
-      </c>
-      <c r="N15" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>2</v>
-      </c>
-      <c r="B16" t="s">
-        <v>69</v>
-      </c>
-      <c r="C16" t="s">
-        <v>70</v>
-      </c>
-      <c r="D16" t="s">
-        <v>62</v>
-      </c>
-      <c r="E16" t="s">
-        <v>70</v>
-      </c>
-      <c r="F16" t="s">
-        <v>71</v>
-      </c>
-      <c r="N16" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>1</v>
-      </c>
-      <c r="B17" t="s">
-        <v>171</v>
-      </c>
-      <c r="C17" t="s">
-        <v>173</v>
-      </c>
-      <c r="D17" t="s">
-        <v>172</v>
-      </c>
-      <c r="E17" t="s">
-        <v>173</v>
-      </c>
-      <c r="F17" t="s">
-        <v>174</v>
-      </c>
-      <c r="N17" s="1" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D17" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="O17" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="P17" s="3" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>73</v>
+        <v>180</v>
       </c>
       <c r="C18" t="s">
-        <v>74</v>
+        <v>43</v>
       </c>
       <c r="D18" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="E18" t="s">
-        <v>74</v>
+        <v>45</v>
       </c>
       <c r="F18" t="s">
-        <v>75</v>
-      </c>
-      <c r="N18" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+      <c r="G18" t="s">
+        <v>46</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>1</v>
       </c>
-      <c r="B19" t="s">
-        <v>186</v>
+      <c r="B19" s="2" t="s">
+        <v>180</v>
       </c>
       <c r="C19" t="s">
-        <v>187</v>
+        <v>138</v>
       </c>
       <c r="D19" t="s">
-        <v>188</v>
+        <v>140</v>
       </c>
       <c r="E19" t="s">
-        <v>187</v>
+        <v>139</v>
       </c>
       <c r="F19" t="s">
-        <v>189</v>
-      </c>
-      <c r="N19" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+        <v>140</v>
+      </c>
+      <c r="G19" t="s">
+        <v>141</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>77</v>
+        <v>179</v>
       </c>
       <c r="C20" t="s">
-        <v>78</v>
+        <v>48</v>
       </c>
       <c r="D20" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E20" t="s">
-        <v>78</v>
+        <v>50</v>
       </c>
       <c r="F20" t="s">
-        <v>79</v>
-      </c>
-      <c r="N20" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+      <c r="G20" t="s">
+        <v>51</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>1</v>
       </c>
-      <c r="B21" t="s">
-        <v>81</v>
+      <c r="B21" s="2" t="s">
+        <v>180</v>
       </c>
       <c r="C21" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="D21" t="s">
-        <v>8</v>
+        <v>68</v>
       </c>
       <c r="E21" t="s">
-        <v>82</v>
-      </c>
-      <c r="H21" t="s">
-        <v>82</v>
-      </c>
-      <c r="N21" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+      <c r="F21" t="s">
+        <v>68</v>
+      </c>
+      <c r="I21" t="s">
+        <v>68</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>1</v>
       </c>
-      <c r="B22" t="s">
-        <v>84</v>
+      <c r="B22" s="2" t="s">
+        <v>180</v>
       </c>
       <c r="C22" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="D22" t="s">
-        <v>8</v>
+        <v>71</v>
       </c>
       <c r="E22" t="s">
-        <v>86</v>
-      </c>
-      <c r="H22" t="s">
-        <v>86</v>
-      </c>
-      <c r="N22" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+      <c r="F22" t="s">
+        <v>71</v>
+      </c>
+      <c r="I22" t="s">
+        <v>71</v>
+      </c>
+      <c r="O22" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>1</v>
       </c>
-      <c r="B23" t="s">
-        <v>88</v>
+      <c r="B23" s="2" t="s">
+        <v>180</v>
       </c>
       <c r="C23" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="D23" t="s">
-        <v>9</v>
+        <v>74</v>
       </c>
       <c r="E23" t="s">
-        <v>89</v>
-      </c>
-      <c r="I23" t="s">
-        <v>89</v>
-      </c>
-      <c r="N23" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+      <c r="F23" t="s">
+        <v>74</v>
+      </c>
+      <c r="J23" t="s">
+        <v>74</v>
+      </c>
+      <c r="O23" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="P23" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>4</v>
       </c>
-      <c r="B24" t="s">
-        <v>91</v>
+      <c r="B24" s="2" t="s">
+        <v>180</v>
       </c>
       <c r="C24" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="D24" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="E24" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="F24" t="s">
-        <v>94</v>
-      </c>
-      <c r="N24" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A25">
+        <v>77</v>
+      </c>
+      <c r="G24" t="s">
+        <v>79</v>
+      </c>
+      <c r="O24" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="P24" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="2">
         <v>4</v>
       </c>
-      <c r="B25" t="s">
-        <v>96</v>
-      </c>
-      <c r="C25" t="s">
-        <v>97</v>
-      </c>
-      <c r="D25" t="s">
-        <v>98</v>
-      </c>
-      <c r="E25" t="s">
-        <v>97</v>
-      </c>
-      <c r="F25" t="s">
-        <v>99</v>
-      </c>
-      <c r="G25" t="s">
-        <v>100</v>
-      </c>
-      <c r="N25" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B25" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="O25" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="P25" s="3" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>6</v>
       </c>
-      <c r="B26" t="s">
-        <v>102</v>
+      <c r="B26" s="2" t="s">
+        <v>180</v>
       </c>
       <c r="C26" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="D26" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="E26" t="s">
-        <v>103</v>
-      </c>
-      <c r="J26" t="s">
-        <v>103</v>
-      </c>
-      <c r="N26" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+      <c r="F26" t="s">
+        <v>82</v>
+      </c>
+      <c r="K26" t="s">
+        <v>82</v>
+      </c>
+      <c r="O26" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="P26" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>2</v>
       </c>
-      <c r="B27" t="s">
-        <v>106</v>
+      <c r="B27" s="2" t="s">
+        <v>180</v>
       </c>
       <c r="C27" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
       <c r="D27" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="E27" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="F27" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="G27" t="s">
-        <v>107</v>
-      </c>
-      <c r="N27" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+      <c r="H27" t="s">
+        <v>224</v>
+      </c>
+      <c r="O27" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="P27" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>2</v>
       </c>
-      <c r="B28" t="s">
-        <v>111</v>
+      <c r="B28" s="2" t="s">
+        <v>180</v>
       </c>
       <c r="C28" t="s">
-        <v>112</v>
+        <v>85</v>
       </c>
       <c r="D28" t="s">
-        <v>108</v>
+        <v>86</v>
       </c>
       <c r="E28" t="s">
-        <v>112</v>
+        <v>87</v>
       </c>
       <c r="F28" t="s">
-        <v>113</v>
+        <v>86</v>
       </c>
       <c r="G28" t="s">
-        <v>112</v>
-      </c>
-      <c r="N28" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+      <c r="H28" t="s">
+        <v>225</v>
+      </c>
+      <c r="O28" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="P28" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>1</v>
       </c>
-      <c r="B29" t="s">
-        <v>115</v>
+      <c r="B29" s="2" t="s">
+        <v>180</v>
       </c>
       <c r="C29" t="s">
-        <v>116</v>
+        <v>94</v>
       </c>
       <c r="D29" t="s">
-        <v>117</v>
+        <v>95</v>
       </c>
       <c r="E29" t="s">
-        <v>116</v>
-      </c>
-      <c r="I29" t="s">
-        <v>116</v>
-      </c>
-      <c r="N29" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A30">
+        <v>96</v>
+      </c>
+      <c r="F29" t="s">
+        <v>95</v>
+      </c>
+      <c r="J29" t="s">
+        <v>95</v>
+      </c>
+      <c r="O29" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="P29" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="2">
         <v>4</v>
       </c>
-      <c r="B30" t="s">
-        <v>119</v>
-      </c>
-      <c r="C30" t="s">
-        <v>120</v>
-      </c>
-      <c r="D30" t="s">
-        <v>57</v>
-      </c>
-      <c r="E30" t="s">
-        <v>120</v>
-      </c>
-      <c r="F30" t="s">
-        <v>121</v>
-      </c>
-      <c r="G30" t="s">
-        <v>120</v>
-      </c>
-      <c r="N30" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B30" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="O30" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="P30" s="3" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>4</v>
       </c>
-      <c r="B31" t="s">
-        <v>123</v>
+      <c r="B31" s="2" t="s">
+        <v>180</v>
       </c>
       <c r="C31" t="s">
-        <v>124</v>
+        <v>99</v>
       </c>
       <c r="D31" t="s">
-        <v>125</v>
+        <v>100</v>
       </c>
       <c r="E31" t="s">
-        <v>124</v>
+        <v>101</v>
       </c>
       <c r="F31" t="s">
-        <v>126</v>
-      </c>
-      <c r="N31" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+      <c r="G31" t="s">
+        <v>102</v>
+      </c>
+      <c r="O31" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="P31" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>1</v>
       </c>
-      <c r="B32" t="s">
-        <v>128</v>
+      <c r="B32" s="2" t="s">
+        <v>180</v>
       </c>
       <c r="C32" t="s">
-        <v>129</v>
+        <v>103</v>
       </c>
       <c r="D32" t="s">
-        <v>130</v>
+        <v>104</v>
       </c>
       <c r="E32" t="s">
-        <v>129</v>
-      </c>
-      <c r="K32" t="s">
-        <v>129</v>
-      </c>
-      <c r="N32" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+      <c r="F32" t="s">
+        <v>104</v>
+      </c>
+      <c r="L32" t="s">
+        <v>104</v>
+      </c>
+      <c r="O32" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="P32" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>1</v>
       </c>
-      <c r="B33" t="s">
-        <v>132</v>
+      <c r="B33" s="2" t="s">
+        <v>180</v>
       </c>
       <c r="C33" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="D33" t="s">
-        <v>134</v>
+        <v>108</v>
       </c>
       <c r="E33" t="s">
-        <v>133</v>
+        <v>109</v>
       </c>
       <c r="F33" t="s">
-        <v>135</v>
+        <v>108</v>
       </c>
       <c r="G33" t="s">
-        <v>133</v>
-      </c>
-      <c r="N33" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+      <c r="H33" t="s">
+        <v>227</v>
+      </c>
+      <c r="O33" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="P33" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>1</v>
       </c>
-      <c r="B34" t="s">
-        <v>137</v>
+      <c r="B34" s="2" t="s">
+        <v>180</v>
       </c>
       <c r="C34" t="s">
-        <v>138</v>
+        <v>112</v>
       </c>
       <c r="D34" t="s">
-        <v>139</v>
+        <v>113</v>
       </c>
       <c r="E34" t="s">
-        <v>138</v>
-      </c>
-      <c r="L34" t="s">
-        <v>140</v>
-      </c>
-      <c r="N34" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+        <v>114</v>
+      </c>
+      <c r="F34" t="s">
+        <v>113</v>
+      </c>
+      <c r="M34" t="s">
+        <v>115</v>
+      </c>
+      <c r="O34" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="P34" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>1</v>
       </c>
-      <c r="B35" t="s">
-        <v>142</v>
+      <c r="B35" s="2" t="s">
+        <v>180</v>
       </c>
       <c r="C35" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="D35" t="s">
-        <v>144</v>
+        <v>128</v>
       </c>
       <c r="E35" t="s">
-        <v>143</v>
-      </c>
-      <c r="M35" t="s">
-        <v>142</v>
-      </c>
-      <c r="N35" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+        <v>129</v>
+      </c>
+      <c r="F35" t="s">
+        <v>128</v>
+      </c>
+      <c r="N35" t="s">
+        <v>128</v>
+      </c>
+      <c r="O35" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="P35" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>1</v>
       </c>
-      <c r="B36" t="s">
-        <v>146</v>
+      <c r="B36" s="2" t="s">
+        <v>180</v>
       </c>
       <c r="C36" t="s">
-        <v>146</v>
+        <v>117</v>
       </c>
       <c r="D36" t="s">
-        <v>147</v>
+        <v>118</v>
       </c>
       <c r="E36" t="s">
-        <v>146</v>
-      </c>
-      <c r="M36" t="s">
-        <v>148</v>
-      </c>
-      <c r="N36" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+        <v>119</v>
+      </c>
+      <c r="F36" t="s">
+        <v>118</v>
+      </c>
+      <c r="N36" t="s">
+        <v>117</v>
+      </c>
+      <c r="O36" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="P36" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>1</v>
       </c>
-      <c r="B37" t="s">
-        <v>150</v>
+      <c r="B37" s="2" t="s">
+        <v>180</v>
       </c>
       <c r="C37" t="s">
-        <v>151</v>
+        <v>120</v>
       </c>
       <c r="D37" t="s">
-        <v>152</v>
+        <v>120</v>
       </c>
       <c r="E37" t="s">
-        <v>151</v>
+        <v>121</v>
       </c>
       <c r="F37" t="s">
-        <v>153</v>
-      </c>
-      <c r="G37" t="s">
-        <v>151</v>
-      </c>
-      <c r="N37" s="1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+        <v>120</v>
+      </c>
+      <c r="N37" t="s">
+        <v>122</v>
+      </c>
+      <c r="O37" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="P37" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>1</v>
       </c>
-      <c r="B38" t="s">
-        <v>155</v>
+      <c r="B38" s="2" t="s">
+        <v>180</v>
       </c>
       <c r="C38" t="s">
-        <v>156</v>
+        <v>123</v>
       </c>
       <c r="D38" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="E38" t="s">
-        <v>156</v>
-      </c>
-      <c r="M38" t="s">
-        <v>155</v>
-      </c>
-      <c r="N38" s="1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+      <c r="F38" t="s">
+        <v>143</v>
+      </c>
+      <c r="G38" t="s">
+        <v>144</v>
+      </c>
+      <c r="H38" t="s">
+        <v>218</v>
+      </c>
+      <c r="O38" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="P38" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39">
-        <v>1</v>
-      </c>
-      <c r="B39" t="s">
-        <v>159</v>
+        <v>10</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>180</v>
       </c>
       <c r="C39" t="s">
-        <v>160</v>
+        <v>130</v>
       </c>
       <c r="D39" t="s">
-        <v>161</v>
+        <v>131</v>
       </c>
       <c r="E39" t="s">
-        <v>160</v>
+        <v>132</v>
+      </c>
+      <c r="F39" t="s">
+        <v>131</v>
       </c>
       <c r="M39" t="s">
-        <v>160</v>
-      </c>
-      <c r="N39" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+      <c r="O39" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="P39" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>1</v>
       </c>
       <c r="B40" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="C40" t="s">
-        <v>178</v>
+        <v>124</v>
       </c>
       <c r="D40" t="s">
+        <v>125</v>
+      </c>
+      <c r="E40" t="s">
+        <v>126</v>
+      </c>
+      <c r="F40" t="s">
+        <v>125</v>
+      </c>
+      <c r="N40" t="s">
+        <v>124</v>
+      </c>
+      <c r="O40" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="P40" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>1</v>
+      </c>
+      <c r="B41" t="s">
         <v>179</v>
       </c>
-      <c r="E40" t="s">
-        <v>178</v>
-      </c>
-      <c r="F40" t="s">
-        <v>180</v>
-      </c>
-      <c r="G40" t="s">
-        <v>181</v>
-      </c>
-      <c r="N40" s="1" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A41">
-        <v>10</v>
-      </c>
-      <c r="B41" t="s">
-        <v>163</v>
-      </c>
       <c r="C41" t="s">
-        <v>164</v>
+        <v>16</v>
       </c>
       <c r="D41" t="s">
-        <v>165</v>
+        <v>17</v>
       </c>
       <c r="E41" t="s">
-        <v>164</v>
-      </c>
-      <c r="L41" t="s">
-        <v>166</v>
-      </c>
-      <c r="N41" s="1" t="s">
-        <v>167</v>
+        <v>18</v>
+      </c>
+      <c r="F41" t="s">
+        <v>17</v>
+      </c>
+      <c r="G41" t="s">
+        <v>19</v>
+      </c>
+      <c r="O41" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P41" s="1" t="s">
+        <v>215</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="N7" r:id="rId1"/>
-    <hyperlink ref="N6" r:id="rId2"/>
-    <hyperlink ref="N5" r:id="rId3"/>
-    <hyperlink ref="N4" r:id="rId4"/>
-    <hyperlink ref="N8" r:id="rId5"/>
-    <hyperlink ref="N17" r:id="rId6"/>
-    <hyperlink ref="N9" r:id="rId7"/>
-    <hyperlink ref="N10" r:id="rId8"/>
-    <hyperlink ref="N11" r:id="rId9"/>
-    <hyperlink ref="N12" r:id="rId10"/>
-    <hyperlink ref="N13" r:id="rId11"/>
-    <hyperlink ref="N14" r:id="rId12"/>
-    <hyperlink ref="N15" r:id="rId13"/>
-    <hyperlink ref="N16" r:id="rId14"/>
-    <hyperlink ref="N18" r:id="rId15"/>
-    <hyperlink ref="N19" r:id="rId16"/>
-    <hyperlink ref="N20" r:id="rId17"/>
-    <hyperlink ref="N21" r:id="rId18"/>
-    <hyperlink ref="N22" r:id="rId19"/>
-    <hyperlink ref="N23" r:id="rId20"/>
-    <hyperlink ref="N24" r:id="rId21"/>
-    <hyperlink ref="N25" r:id="rId22"/>
-    <hyperlink ref="N26" r:id="rId23"/>
-    <hyperlink ref="N27" r:id="rId24"/>
-    <hyperlink ref="N28" r:id="rId25"/>
-    <hyperlink ref="N29" r:id="rId26"/>
-    <hyperlink ref="N30" r:id="rId27"/>
-    <hyperlink ref="N31" r:id="rId28"/>
-    <hyperlink ref="N32" r:id="rId29"/>
-    <hyperlink ref="N33" r:id="rId30"/>
-    <hyperlink ref="N34" r:id="rId31"/>
-    <hyperlink ref="N35" r:id="rId32"/>
-    <hyperlink ref="N36" r:id="rId33"/>
-    <hyperlink ref="N37" r:id="rId34"/>
-    <hyperlink ref="N38" r:id="rId35"/>
-    <hyperlink ref="N39" r:id="rId36"/>
-    <hyperlink ref="N41" r:id="rId37"/>
-    <hyperlink ref="N3" r:id="rId38"/>
-    <hyperlink ref="N40" r:id="rId39"/>
+    <hyperlink ref="O5" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="O7" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="O41" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="O6" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="O19" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="O10" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="O8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="O9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="O18" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="O20" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="O14" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="O12" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="O11" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="O15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="O16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="O17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="O21" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="O22" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="O23" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="O24" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="O25" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="O26" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="O28" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="O27" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="O29" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="O30" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="O31" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="O32" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="O33" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="O34" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="O37" r:id="rId31" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="O38" r:id="rId32" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="O40" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="O35" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="O39" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="O3" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="O4" r:id="rId37" xr:uid="{187821FF-BB94-4CF3-9534-31391AA60372}"/>
+    <hyperlink ref="O13" r:id="rId38" xr:uid="{E92330C1-8728-44F5-B45F-7994E19A4C82}"/>
+    <hyperlink ref="P3" r:id="rId39" xr:uid="{16204C99-4F84-41F2-973F-9D15840490A4}"/>
+    <hyperlink ref="P4" r:id="rId40" xr:uid="{C53FE3FE-7E6D-43A0-9FC5-7EFBDC042473}"/>
+    <hyperlink ref="P5" r:id="rId41" xr:uid="{66DEC44C-2FE4-42A6-8F41-7EFF6D7F737E}"/>
+    <hyperlink ref="P6" r:id="rId42" xr:uid="{69715C98-0EE5-4715-8CAA-88C6148C13CE}"/>
+    <hyperlink ref="P7" r:id="rId43" xr:uid="{E94B3599-4F0E-4293-A7CD-B31F50AE8971}"/>
+    <hyperlink ref="P8" r:id="rId44" xr:uid="{4F15A29C-AB4A-4112-97E5-0B95D72568B0}"/>
+    <hyperlink ref="P9" r:id="rId45" xr:uid="{952DF9DF-1114-490B-B564-1E33CC1C39A0}"/>
+    <hyperlink ref="P10" r:id="rId46" xr:uid="{9768116C-FFCA-4905-8394-C5DABAA20429}"/>
+    <hyperlink ref="P11" r:id="rId47" xr:uid="{7E1A165F-EEA4-413A-928F-65ED60B462AC}"/>
+    <hyperlink ref="P12" r:id="rId48" display="https://www.digikey.ca/product-detail/en/molex-connector-corporation/22-05-2031/WM4101-ND/" xr:uid="{6473195A-FA32-4522-B836-6BF5F9E606FC}"/>
+    <hyperlink ref="P13" r:id="rId49" display="https://www.digikey.ca/product-detail/en/preci-dip/801-87-003-10-001101/1212-1180-ND" xr:uid="{D7AF70A9-C39C-4905-83E6-2DA90434F9DE}"/>
+    <hyperlink ref="P14" r:id="rId50" xr:uid="{235DABA3-40CF-4E7F-BE96-6E4C7BD762FF}"/>
+    <hyperlink ref="P15" r:id="rId51" xr:uid="{711F3DA8-4E78-48E0-92BE-13892D79E1BD}"/>
+    <hyperlink ref="P16" r:id="rId52" display="https://www.digikey.ca/product-detail/en/everlight-electronics-co-ltd/MV5437/1080-1109-ND/2675600" xr:uid="{3577F028-31D3-499F-A397-533479D011C7}"/>
+    <hyperlink ref="P17" r:id="rId53" display="https://www.digikey.ca/product-detail/en/sullins-connector-solutions/SPC02SYAN/S9002-ND" xr:uid="{BBF4E608-666B-41AA-8521-CF516DC539D0}"/>
+    <hyperlink ref="P18" r:id="rId54" display="http://www.digikey.ca/product-detail/en/fairchild-on-semiconductor/2N3906TFR/2N3906D26ZCT-ND" xr:uid="{B741301F-5F09-4977-ACBD-FE728D0CD341}"/>
+    <hyperlink ref="P19" r:id="rId55" display="https://www.digikey.ca/product-detail/en/sullins-connector-solutions/PPPC061LFBN-RC/S7039-ND" xr:uid="{B022C9C9-0264-481E-BB22-5F7D88341532}"/>
+    <hyperlink ref="P20" r:id="rId56" display="http://www.digikey.ca/product-detail/en/3m/929974-01-01/929974-01-01-ND" xr:uid="{5E5BA37D-12C2-4EC5-8231-8BAFD90FF127}"/>
+    <hyperlink ref="P21" r:id="rId57" xr:uid="{580A9C0D-596A-41DC-94A7-573E76C63E2A}"/>
+    <hyperlink ref="P22" r:id="rId58" xr:uid="{84332E5C-93DC-4F84-8A05-9651D10ADEE8}"/>
+    <hyperlink ref="P23" r:id="rId59" xr:uid="{2DB69685-885F-4B05-873C-F02DBA4D407E}"/>
+    <hyperlink ref="P24" r:id="rId60" xr:uid="{8B2312DC-55D5-47F1-B414-90C98203CB7C}"/>
+    <hyperlink ref="P25" r:id="rId61" display="https://www.digikey.ca/product-detail/en/essentra-components/NMS-308/RP809-ND" xr:uid="{423744EE-8DD1-463A-884F-A98B77D8798D}"/>
+    <hyperlink ref="P26" r:id="rId62" xr:uid="{25273784-7AE2-451B-9614-59E67B7974AB}"/>
+    <hyperlink ref="P27" r:id="rId63" xr:uid="{88003930-28B1-4638-851F-1E57A532D3B8}"/>
+    <hyperlink ref="P28" r:id="rId64" display="http://www.digikey.ca/product-detail/en/keystone-electronics/25503/36-25503-ND/" xr:uid="{3FB7BF42-904A-4EF0-8163-8038A2B862C4}"/>
+    <hyperlink ref="P29" r:id="rId65" xr:uid="{9AA159F7-CCE1-4765-A04D-C1449B8016D2}"/>
+    <hyperlink ref="P30" r:id="rId66" display="https://www.digikey.ca/product-detail/en/3m/SJ-5003-(BLACK)/SJ5003-0-ND/102573" xr:uid="{55DDD585-06C5-45C8-B4B5-6B5E82037EFF}"/>
+    <hyperlink ref="P31" r:id="rId67" display="https://www.digikey.ca/product-detail/en/b-f-fastener-supply/MHNZ-003/H762-ND/274973" xr:uid="{3532D585-6362-4A94-91C9-DD45AC09DACC}"/>
+    <hyperlink ref="P32" r:id="rId68" xr:uid="{C8E470EA-8B17-4CA9-88E7-7D091F89E07E}"/>
+    <hyperlink ref="P33" r:id="rId69" xr:uid="{C4A4260D-068B-4ADA-9229-62F7939BE120}"/>
+    <hyperlink ref="P34" r:id="rId70" xr:uid="{7A87EA52-DCB2-4511-80A3-12EA109EB55D}"/>
+    <hyperlink ref="P35" r:id="rId71" xr:uid="{F3A05D0C-D502-47FA-8D70-15D5D1A136C8}"/>
+    <hyperlink ref="P36" r:id="rId72" xr:uid="{A8E4922F-C4FC-4112-AD42-B7F8495754C8}"/>
+    <hyperlink ref="P37" r:id="rId73" xr:uid="{8FE4B6A7-F247-421C-9E68-879BABEA7A92}"/>
+    <hyperlink ref="P38" r:id="rId74" xr:uid="{1E5BD645-76CA-4497-A064-1D9DA1CED248}"/>
+    <hyperlink ref="P39" r:id="rId75" xr:uid="{E12706A6-A035-4A67-A6CB-7AABFFD21D46}"/>
+    <hyperlink ref="P40" r:id="rId76" xr:uid="{8CB2FBCA-F517-41A1-8871-75C28A8C8E3C}"/>
+    <hyperlink ref="P41" r:id="rId77" display="http://www.digikey.ca/product-detail/en/sparkfun-electronics/WRL-12576/1568-1265-ND" xr:uid="{A7D5F7CF-ABAE-4098-88BF-486827150AA5}"/>
+    <hyperlink ref="O36" r:id="rId78" xr:uid="{B6661026-2BFB-4FDA-94E3-E45FCAA7538B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated BOM file ( December 13,2017 )
</commit_message>
<xml_diff>
--- a/LipSync_BOM.xlsx
+++ b/LipSync_BOM.xlsx
@@ -1,25 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="26215"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Milad\Development\makersmakingchange\LipSync\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kmok/Documents/NSS/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="13360"/>
   </bookViews>
   <sheets>
     <sheet name="LipSync_BOM" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="229">
   <si>
     <t>Qty</t>
   </si>
@@ -321,15 +326,6 @@
     <t xml:space="preserve">Nut M3 </t>
   </si>
   <si>
-    <t>MHNZ 003</t>
-  </si>
-  <si>
-    <t>Building Fasteners</t>
-  </si>
-  <si>
-    <t>H762-ND</t>
-  </si>
-  <si>
     <t xml:space="preserve">Tubing Tygon 3350 3/32" ID x 45mm </t>
   </si>
   <si>
@@ -450,12 +446,6 @@
     <t>https://www.digikey.ca/product-detail/en/sullins-connector-solutions/PPPC061LFBN-RC/S7039-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">2-604771-9 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2-604771-9-ND </t>
-  </si>
-  <si>
     <t>10k Ohm 1/4W Mini Axial Through-Hole Resistor</t>
   </si>
   <si>
@@ -546,12 +536,6 @@
     <t>https://www.digikey.ca/product-detail/en/3m/SJ-5003-(BLACK)/SJ5003-0-ND/102573</t>
   </si>
   <si>
-    <t>https://www.digikey.ca/product-detail/en/te-connectivity-raychem-cable-protection/2-604771-9/2-604771-9-ND/2259327</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TE Connectivity Raychem </t>
-  </si>
-  <si>
     <t>Component name (October 25,2017)</t>
   </si>
   <si>
@@ -564,9 +548,6 @@
     <t>Required</t>
   </si>
   <si>
-    <t>https://www.digikey.ca/product-detail/en/b-f-fastener-supply/MHNZ-003/H762-ND/274973</t>
-  </si>
-  <si>
     <t>https://www.digikey.ca/product-detail/en/molex-connector-corporation/22-05-2031/WM4101-ND/</t>
   </si>
   <si>
@@ -615,9 +596,6 @@
     <t>https://www.digikey.com/product-detail/en/essentra-components/NMS-308/RP809-ND</t>
   </si>
   <si>
-    <t>https://www.digikey.com/product-detail/en/te-connectivity-raychem-cable-protection/2-604771-9/2-604771-9-ND/2259327</t>
-  </si>
-  <si>
     <t>http://www.digikey.ca/product-detail/en/interlink-electronics/30-49649/1027-1000-ND</t>
   </si>
   <si>
@@ -663,9 +641,6 @@
     <t>https://www.digikey.com/product-detail/en/3m/SJ-5003-(BLACK)/SJ5003-0-ND/102574</t>
   </si>
   <si>
-    <t>https://www.digikey.com/product-detail/en/b-f-fastener-supply/MHNZ-003/H762-ND/274974</t>
-  </si>
-  <si>
     <t>http://www.digikey.com/product-detail/en/sparkfun-electronics/WRL-12576/1568-1265-ND</t>
   </si>
   <si>
@@ -709,12 +684,39 @@
   </si>
   <si>
     <t>https://www.amazon.com/CAMVATE-Female-Male-Piece-Adapter/dp/B01GWVQ022</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/qualtek/17-M100N-M/Q729-ND/4072231</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/qualtek/17-M100N-M/Q729-ND/4072231</t>
+  </si>
+  <si>
+    <t>Q729-ND</t>
+  </si>
+  <si>
+    <t>Qualtek</t>
+  </si>
+  <si>
+    <t>36-4708-ND</t>
+  </si>
+  <si>
+    <t>Keystone Electronics</t>
+  </si>
+  <si>
+    <t>17-M100N-M</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/keystone-electronics/4708/36-4708-ND/4499301</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/keystone-electronics/4708/36-4708-ND/4499301</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1201,11 +1203,14 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1561,32 +1566,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" topLeftCell="D21" workbookViewId="0">
+      <selection activeCell="P31" sqref="P31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="50.5546875" customWidth="1"/>
-    <col min="4" max="4" width="35.44140625" customWidth="1"/>
-    <col min="6" max="6" width="24.88671875" customWidth="1"/>
+    <col min="3" max="3" width="50.5" customWidth="1"/>
+    <col min="4" max="4" width="35.5" customWidth="1"/>
+    <col min="6" max="6" width="24.83203125" customWidth="1"/>
     <col min="7" max="7" width="27.6640625" customWidth="1"/>
-    <col min="8" max="8" width="13.21875" customWidth="1"/>
-    <col min="15" max="15" width="18.77734375" customWidth="1"/>
+    <col min="8" max="8" width="13.1640625" customWidth="1"/>
+    <col min="15" max="15" width="18.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="C1" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -1622,13 +1627,13 @@
         <v>4</v>
       </c>
       <c r="O1" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="P1" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="G2" t="s">
         <v>5</v>
       </c>
@@ -1654,15 +1659,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="C3" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="D3" t="s">
         <v>13</v>
@@ -1674,24 +1679,24 @@
         <v>13</v>
       </c>
       <c r="G3" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="H3" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>15</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="C4" t="s">
         <v>25</v>
@@ -1712,73 +1717,73 @@
         <v>29</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="C5" t="s">
         <v>30</v>
       </c>
       <c r="D5" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E5" t="s">
         <v>31</v>
       </c>
       <c r="F5" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="G5" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="C6" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="D6" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="E6" t="s">
         <v>31</v>
       </c>
       <c r="F6" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="G6" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="C7" t="s">
         <v>21</v>
@@ -1796,53 +1801,53 @@
         <v>24</v>
       </c>
       <c r="H7" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>1</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>37</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>34</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="O8" s="3" t="s">
         <v>38</v>
       </c>
       <c r="P8" s="3" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="C9" t="s">
         <v>39</v>
@@ -1860,21 +1865,21 @@
         <v>41</v>
       </c>
       <c r="H9" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>42</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="C10" t="s">
         <v>32</v>
@@ -1886,27 +1891,27 @@
         <v>34</v>
       </c>
       <c r="F10" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="G10" t="s">
         <v>35</v>
       </c>
       <c r="H10" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="O10" s="1" t="s">
         <v>36</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="C11" t="s">
         <v>58</v>
@@ -1927,73 +1932,73 @@
         <v>61</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>2</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="O12" s="3" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="P12" s="3" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>2</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="O13" s="3" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="P13" s="3" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="C14" t="s">
         <v>53</v>
@@ -2014,15 +2019,15 @@
         <v>57</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="C15" t="s">
         <v>62</v>
@@ -2043,73 +2048,73 @@
         <v>65</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>1</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="O16" s="3" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="P16" s="3" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>1</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>66</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>55</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="O17" s="3" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="P17" s="3" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="C18" t="s">
         <v>43</v>
@@ -2130,44 +2135,44 @@
         <v>47</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="C19" t="s">
+        <v>135</v>
+      </c>
+      <c r="D19" t="s">
+        <v>137</v>
+      </c>
+      <c r="E19" t="s">
+        <v>136</v>
+      </c>
+      <c r="F19" t="s">
+        <v>137</v>
+      </c>
+      <c r="G19" t="s">
         <v>138</v>
       </c>
-      <c r="D19" t="s">
-        <v>140</v>
-      </c>
-      <c r="E19" t="s">
+      <c r="O19" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="F19" t="s">
-        <v>140</v>
-      </c>
-      <c r="G19" t="s">
-        <v>141</v>
-      </c>
-      <c r="O19" s="1" t="s">
-        <v>142</v>
-      </c>
       <c r="P19" s="1" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="C20" t="s">
         <v>48</v>
@@ -2188,15 +2193,15 @@
         <v>52</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="C21" t="s">
         <v>67</v>
@@ -2220,12 +2225,12 @@
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="C22" t="s">
         <v>70</v>
@@ -2249,12 +2254,12 @@
         <v>72</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="C23" t="s">
         <v>73</v>
@@ -2278,12 +2283,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>4</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="C24" t="s">
         <v>76</v>
@@ -2301,47 +2306,47 @@
         <v>79</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="P24" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="25" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>4</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="O25" s="3" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="P25" s="3" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>6</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="C26" t="s">
         <v>81</v>
@@ -2365,12 +2370,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>2</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="C27" t="s">
         <v>90</v>
@@ -2388,21 +2393,21 @@
         <v>92</v>
       </c>
       <c r="H27" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="P27" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>2</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="C28" t="s">
         <v>85</v>
@@ -2420,21 +2425,21 @@
         <v>88</v>
       </c>
       <c r="H28" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="O28" s="1" t="s">
         <v>89</v>
       </c>
       <c r="P28" s="1" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>1</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="C29" t="s">
         <v>94</v>
@@ -2458,340 +2463,340 @@
         <v>97</v>
       </c>
     </row>
-    <row r="30" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>4</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>98</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>50</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="O30" s="3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="P30" s="3" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>4</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="C31" t="s">
         <v>99</v>
       </c>
-      <c r="D31" t="s">
-        <v>100</v>
+      <c r="D31" s="4">
+        <v>4708</v>
       </c>
       <c r="E31" t="s">
-        <v>101</v>
-      </c>
-      <c r="F31" t="s">
-        <v>100</v>
+        <v>225</v>
+      </c>
+      <c r="F31" s="4">
+        <v>4708</v>
       </c>
       <c r="G31" t="s">
-        <v>102</v>
+        <v>224</v>
       </c>
       <c r="O31" s="1" t="s">
-        <v>181</v>
+        <v>227</v>
       </c>
       <c r="P31" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>1</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="C32" t="s">
+        <v>100</v>
+      </c>
+      <c r="D32" t="s">
+        <v>101</v>
+      </c>
+      <c r="E32" t="s">
+        <v>102</v>
+      </c>
+      <c r="F32" t="s">
+        <v>101</v>
+      </c>
+      <c r="L32" t="s">
+        <v>101</v>
+      </c>
+      <c r="O32" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D32" t="s">
-        <v>104</v>
-      </c>
-      <c r="E32" t="s">
-        <v>105</v>
-      </c>
-      <c r="F32" t="s">
-        <v>104</v>
-      </c>
-      <c r="L32" t="s">
-        <v>104</v>
-      </c>
-      <c r="O32" s="1" t="s">
-        <v>106</v>
-      </c>
       <c r="P32" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>1</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="C33" t="s">
+        <v>104</v>
+      </c>
+      <c r="D33" t="s">
+        <v>105</v>
+      </c>
+      <c r="E33" t="s">
+        <v>106</v>
+      </c>
+      <c r="F33" t="s">
+        <v>105</v>
+      </c>
+      <c r="G33" t="s">
         <v>107</v>
       </c>
-      <c r="D33" t="s">
+      <c r="H33" t="s">
+        <v>217</v>
+      </c>
+      <c r="O33" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="E33" t="s">
-        <v>109</v>
-      </c>
-      <c r="F33" t="s">
+      <c r="P33" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="G33" t="s">
-        <v>110</v>
-      </c>
-      <c r="H33" t="s">
-        <v>227</v>
-      </c>
-      <c r="O33" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="P33" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>1</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="C34" t="s">
+        <v>109</v>
+      </c>
+      <c r="D34" t="s">
+        <v>110</v>
+      </c>
+      <c r="E34" t="s">
+        <v>111</v>
+      </c>
+      <c r="F34" t="s">
+        <v>110</v>
+      </c>
+      <c r="M34" t="s">
         <v>112</v>
       </c>
-      <c r="D34" t="s">
+      <c r="O34" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="E34" t="s">
-        <v>114</v>
-      </c>
-      <c r="F34" t="s">
+      <c r="P34" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="M34" t="s">
-        <v>115</v>
-      </c>
-      <c r="O34" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="P34" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>1</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="C35" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D35" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E35" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="F35" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="N35" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="O35" s="1" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="P35" s="1" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>1</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="C36" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D36" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E36" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F36" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="N36" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="O36" s="1" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="P36" s="1" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>1</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="C37" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D37" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E37" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F37" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="N37" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="O37" s="1" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="P37" s="1" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>1</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="C38" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D38" t="s">
-        <v>143</v>
+        <v>226</v>
       </c>
       <c r="E38" t="s">
-        <v>176</v>
+        <v>223</v>
       </c>
       <c r="F38" t="s">
-        <v>143</v>
+        <v>226</v>
       </c>
       <c r="G38" t="s">
-        <v>144</v>
+        <v>222</v>
       </c>
       <c r="H38" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="O38" s="1" t="s">
-        <v>175</v>
+        <v>221</v>
       </c>
       <c r="P38" s="1" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>10</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="C39" t="s">
+        <v>127</v>
+      </c>
+      <c r="D39" t="s">
+        <v>128</v>
+      </c>
+      <c r="E39" t="s">
+        <v>129</v>
+      </c>
+      <c r="F39" t="s">
+        <v>128</v>
+      </c>
+      <c r="M39" t="s">
         <v>130</v>
       </c>
-      <c r="D39" t="s">
+      <c r="O39" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="E39" t="s">
-        <v>132</v>
-      </c>
-      <c r="F39" t="s">
+      <c r="P39" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="M39" t="s">
-        <v>133</v>
-      </c>
-      <c r="O39" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="P39" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>1</v>
       </c>
       <c r="B40" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="C40" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D40" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E40" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F40" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="N40" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="O40" s="1" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="P40" s="1" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>1</v>
       </c>
       <c r="B41" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="C41" t="s">
         <v>16</v>
@@ -2812,89 +2817,88 @@
         <v>20</v>
       </c>
       <c r="P41" s="1" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="O5" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="O7" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="O41" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="O6" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="O19" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="O10" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="O8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="O9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="O18" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="O20" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="O14" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="O12" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="O11" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="O15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="O16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="O17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="O21" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="O22" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="O23" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="O24" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="O25" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="O26" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="O28" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="O27" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="O29" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="O30" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="O31" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="O32" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="O33" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="O34" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="O37" r:id="rId31" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="O38" r:id="rId32" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="O40" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="O35" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="O39" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="O3" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="O4" r:id="rId37" xr:uid="{187821FF-BB94-4CF3-9534-31391AA60372}"/>
-    <hyperlink ref="O13" r:id="rId38" xr:uid="{E92330C1-8728-44F5-B45F-7994E19A4C82}"/>
-    <hyperlink ref="P3" r:id="rId39" xr:uid="{16204C99-4F84-41F2-973F-9D15840490A4}"/>
-    <hyperlink ref="P4" r:id="rId40" xr:uid="{C53FE3FE-7E6D-43A0-9FC5-7EFBDC042473}"/>
-    <hyperlink ref="P5" r:id="rId41" xr:uid="{66DEC44C-2FE4-42A6-8F41-7EFF6D7F737E}"/>
-    <hyperlink ref="P6" r:id="rId42" xr:uid="{69715C98-0EE5-4715-8CAA-88C6148C13CE}"/>
-    <hyperlink ref="P7" r:id="rId43" xr:uid="{E94B3599-4F0E-4293-A7CD-B31F50AE8971}"/>
-    <hyperlink ref="P8" r:id="rId44" xr:uid="{4F15A29C-AB4A-4112-97E5-0B95D72568B0}"/>
-    <hyperlink ref="P9" r:id="rId45" xr:uid="{952DF9DF-1114-490B-B564-1E33CC1C39A0}"/>
-    <hyperlink ref="P10" r:id="rId46" xr:uid="{9768116C-FFCA-4905-8394-C5DABAA20429}"/>
-    <hyperlink ref="P11" r:id="rId47" xr:uid="{7E1A165F-EEA4-413A-928F-65ED60B462AC}"/>
-    <hyperlink ref="P12" r:id="rId48" display="https://www.digikey.ca/product-detail/en/molex-connector-corporation/22-05-2031/WM4101-ND/" xr:uid="{6473195A-FA32-4522-B836-6BF5F9E606FC}"/>
-    <hyperlink ref="P13" r:id="rId49" display="https://www.digikey.ca/product-detail/en/preci-dip/801-87-003-10-001101/1212-1180-ND" xr:uid="{D7AF70A9-C39C-4905-83E6-2DA90434F9DE}"/>
-    <hyperlink ref="P14" r:id="rId50" xr:uid="{235DABA3-40CF-4E7F-BE96-6E4C7BD762FF}"/>
-    <hyperlink ref="P15" r:id="rId51" xr:uid="{711F3DA8-4E78-48E0-92BE-13892D79E1BD}"/>
-    <hyperlink ref="P16" r:id="rId52" display="https://www.digikey.ca/product-detail/en/everlight-electronics-co-ltd/MV5437/1080-1109-ND/2675600" xr:uid="{3577F028-31D3-499F-A397-533479D011C7}"/>
-    <hyperlink ref="P17" r:id="rId53" display="https://www.digikey.ca/product-detail/en/sullins-connector-solutions/SPC02SYAN/S9002-ND" xr:uid="{BBF4E608-666B-41AA-8521-CF516DC539D0}"/>
-    <hyperlink ref="P18" r:id="rId54" display="http://www.digikey.ca/product-detail/en/fairchild-on-semiconductor/2N3906TFR/2N3906D26ZCT-ND" xr:uid="{B741301F-5F09-4977-ACBD-FE728D0CD341}"/>
-    <hyperlink ref="P19" r:id="rId55" display="https://www.digikey.ca/product-detail/en/sullins-connector-solutions/PPPC061LFBN-RC/S7039-ND" xr:uid="{B022C9C9-0264-481E-BB22-5F7D88341532}"/>
-    <hyperlink ref="P20" r:id="rId56" display="http://www.digikey.ca/product-detail/en/3m/929974-01-01/929974-01-01-ND" xr:uid="{5E5BA37D-12C2-4EC5-8231-8BAFD90FF127}"/>
-    <hyperlink ref="P21" r:id="rId57" xr:uid="{580A9C0D-596A-41DC-94A7-573E76C63E2A}"/>
-    <hyperlink ref="P22" r:id="rId58" xr:uid="{84332E5C-93DC-4F84-8A05-9651D10ADEE8}"/>
-    <hyperlink ref="P23" r:id="rId59" xr:uid="{2DB69685-885F-4B05-873C-F02DBA4D407E}"/>
-    <hyperlink ref="P24" r:id="rId60" xr:uid="{8B2312DC-55D5-47F1-B414-90C98203CB7C}"/>
-    <hyperlink ref="P25" r:id="rId61" display="https://www.digikey.ca/product-detail/en/essentra-components/NMS-308/RP809-ND" xr:uid="{423744EE-8DD1-463A-884F-A98B77D8798D}"/>
-    <hyperlink ref="P26" r:id="rId62" xr:uid="{25273784-7AE2-451B-9614-59E67B7974AB}"/>
-    <hyperlink ref="P27" r:id="rId63" xr:uid="{88003930-28B1-4638-851F-1E57A532D3B8}"/>
-    <hyperlink ref="P28" r:id="rId64" display="http://www.digikey.ca/product-detail/en/keystone-electronics/25503/36-25503-ND/" xr:uid="{3FB7BF42-904A-4EF0-8163-8038A2B862C4}"/>
-    <hyperlink ref="P29" r:id="rId65" xr:uid="{9AA159F7-CCE1-4765-A04D-C1449B8016D2}"/>
-    <hyperlink ref="P30" r:id="rId66" display="https://www.digikey.ca/product-detail/en/3m/SJ-5003-(BLACK)/SJ5003-0-ND/102573" xr:uid="{55DDD585-06C5-45C8-B4B5-6B5E82037EFF}"/>
-    <hyperlink ref="P31" r:id="rId67" display="https://www.digikey.ca/product-detail/en/b-f-fastener-supply/MHNZ-003/H762-ND/274973" xr:uid="{3532D585-6362-4A94-91C9-DD45AC09DACC}"/>
-    <hyperlink ref="P32" r:id="rId68" xr:uid="{C8E470EA-8B17-4CA9-88E7-7D091F89E07E}"/>
-    <hyperlink ref="P33" r:id="rId69" xr:uid="{C4A4260D-068B-4ADA-9229-62F7939BE120}"/>
-    <hyperlink ref="P34" r:id="rId70" xr:uid="{7A87EA52-DCB2-4511-80A3-12EA109EB55D}"/>
-    <hyperlink ref="P35" r:id="rId71" xr:uid="{F3A05D0C-D502-47FA-8D70-15D5D1A136C8}"/>
-    <hyperlink ref="P36" r:id="rId72" xr:uid="{A8E4922F-C4FC-4112-AD42-B7F8495754C8}"/>
-    <hyperlink ref="P37" r:id="rId73" xr:uid="{8FE4B6A7-F247-421C-9E68-879BABEA7A92}"/>
-    <hyperlink ref="P38" r:id="rId74" xr:uid="{1E5BD645-76CA-4497-A064-1D9DA1CED248}"/>
-    <hyperlink ref="P39" r:id="rId75" xr:uid="{E12706A6-A035-4A67-A6CB-7AABFFD21D46}"/>
-    <hyperlink ref="P40" r:id="rId76" xr:uid="{8CB2FBCA-F517-41A1-8871-75C28A8C8E3C}"/>
-    <hyperlink ref="P41" r:id="rId77" display="http://www.digikey.ca/product-detail/en/sparkfun-electronics/WRL-12576/1568-1265-ND" xr:uid="{A7D5F7CF-ABAE-4098-88BF-486827150AA5}"/>
-    <hyperlink ref="O36" r:id="rId78" xr:uid="{B6661026-2BFB-4FDA-94E3-E45FCAA7538B}"/>
+    <hyperlink ref="O5" r:id="rId1"/>
+    <hyperlink ref="O7" r:id="rId2"/>
+    <hyperlink ref="O41" r:id="rId3"/>
+    <hyperlink ref="O6" r:id="rId4"/>
+    <hyperlink ref="O19" r:id="rId5"/>
+    <hyperlink ref="O10" r:id="rId6"/>
+    <hyperlink ref="O8" r:id="rId7"/>
+    <hyperlink ref="O9" r:id="rId8"/>
+    <hyperlink ref="O18" r:id="rId9"/>
+    <hyperlink ref="O20" r:id="rId10"/>
+    <hyperlink ref="O14" r:id="rId11"/>
+    <hyperlink ref="O12" r:id="rId12"/>
+    <hyperlink ref="O11" r:id="rId13"/>
+    <hyperlink ref="O15" r:id="rId14"/>
+    <hyperlink ref="O16" r:id="rId15"/>
+    <hyperlink ref="O17" r:id="rId16"/>
+    <hyperlink ref="O21" r:id="rId17"/>
+    <hyperlink ref="O22" r:id="rId18"/>
+    <hyperlink ref="O23" r:id="rId19"/>
+    <hyperlink ref="O24" r:id="rId20"/>
+    <hyperlink ref="O25" r:id="rId21"/>
+    <hyperlink ref="O26" r:id="rId22"/>
+    <hyperlink ref="O28" r:id="rId23"/>
+    <hyperlink ref="O27" r:id="rId24"/>
+    <hyperlink ref="O29" r:id="rId25"/>
+    <hyperlink ref="O30" r:id="rId26"/>
+    <hyperlink ref="O31" r:id="rId27"/>
+    <hyperlink ref="O32" r:id="rId28"/>
+    <hyperlink ref="O33" r:id="rId29"/>
+    <hyperlink ref="O34" r:id="rId30"/>
+    <hyperlink ref="O37" r:id="rId31"/>
+    <hyperlink ref="O40" r:id="rId32"/>
+    <hyperlink ref="O35" r:id="rId33"/>
+    <hyperlink ref="O39" r:id="rId34"/>
+    <hyperlink ref="O3" r:id="rId35"/>
+    <hyperlink ref="O4" r:id="rId36"/>
+    <hyperlink ref="O13" r:id="rId37"/>
+    <hyperlink ref="P3" r:id="rId38"/>
+    <hyperlink ref="P4" r:id="rId39"/>
+    <hyperlink ref="P5" r:id="rId40"/>
+    <hyperlink ref="P6" r:id="rId41"/>
+    <hyperlink ref="P7" r:id="rId42"/>
+    <hyperlink ref="P8" r:id="rId43"/>
+    <hyperlink ref="P9" r:id="rId44"/>
+    <hyperlink ref="P10" r:id="rId45"/>
+    <hyperlink ref="P11" r:id="rId46"/>
+    <hyperlink ref="P12" r:id="rId47" display="https://www.digikey.ca/product-detail/en/molex-connector-corporation/22-05-2031/WM4101-ND/"/>
+    <hyperlink ref="P13" r:id="rId48" display="https://www.digikey.ca/product-detail/en/preci-dip/801-87-003-10-001101/1212-1180-ND"/>
+    <hyperlink ref="P14" r:id="rId49"/>
+    <hyperlink ref="P15" r:id="rId50"/>
+    <hyperlink ref="P16" r:id="rId51" display="https://www.digikey.ca/product-detail/en/everlight-electronics-co-ltd/MV5437/1080-1109-ND/2675600"/>
+    <hyperlink ref="P17" r:id="rId52" display="https://www.digikey.ca/product-detail/en/sullins-connector-solutions/SPC02SYAN/S9002-ND"/>
+    <hyperlink ref="P18" r:id="rId53" display="http://www.digikey.ca/product-detail/en/fairchild-on-semiconductor/2N3906TFR/2N3906D26ZCT-ND"/>
+    <hyperlink ref="P19" r:id="rId54" display="https://www.digikey.ca/product-detail/en/sullins-connector-solutions/PPPC061LFBN-RC/S7039-ND"/>
+    <hyperlink ref="P20" r:id="rId55" display="http://www.digikey.ca/product-detail/en/3m/929974-01-01/929974-01-01-ND"/>
+    <hyperlink ref="P21" r:id="rId56"/>
+    <hyperlink ref="P22" r:id="rId57"/>
+    <hyperlink ref="P23" r:id="rId58"/>
+    <hyperlink ref="P24" r:id="rId59"/>
+    <hyperlink ref="P25" r:id="rId60" display="https://www.digikey.ca/product-detail/en/essentra-components/NMS-308/RP809-ND"/>
+    <hyperlink ref="P26" r:id="rId61"/>
+    <hyperlink ref="P27" r:id="rId62"/>
+    <hyperlink ref="P28" r:id="rId63" display="http://www.digikey.ca/product-detail/en/keystone-electronics/25503/36-25503-ND/"/>
+    <hyperlink ref="P29" r:id="rId64"/>
+    <hyperlink ref="P30" r:id="rId65" display="https://www.digikey.ca/product-detail/en/3m/SJ-5003-(BLACK)/SJ5003-0-ND/102573"/>
+    <hyperlink ref="P31" r:id="rId66"/>
+    <hyperlink ref="P32" r:id="rId67"/>
+    <hyperlink ref="P33" r:id="rId68"/>
+    <hyperlink ref="P34" r:id="rId69"/>
+    <hyperlink ref="P35" r:id="rId70"/>
+    <hyperlink ref="P36" r:id="rId71"/>
+    <hyperlink ref="P37" r:id="rId72"/>
+    <hyperlink ref="P39" r:id="rId73"/>
+    <hyperlink ref="P40" r:id="rId74"/>
+    <hyperlink ref="P41" r:id="rId75" display="http://www.digikey.ca/product-detail/en/sparkfun-electronics/WRL-12576/1568-1265-ND"/>
+    <hyperlink ref="O36" r:id="rId76"/>
+    <hyperlink ref="O38" r:id="rId77"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated BOM file (March 2, 2018)
</commit_message>
<xml_diff>
--- a/LipSync_BOM.xlsx
+++ b/LipSync_BOM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="228">
   <si>
     <t>Qty</t>
   </si>
@@ -650,9 +650,6 @@
     <t>https://www.digikey.com/product-detail/en/freescale-semiconductor-nxp/MPXV7002DPT1/MPXV7002DPT1CT-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">571-2-604771-9 </t>
-  </si>
-  <si>
     <t>80-C315C103K5R</t>
   </si>
   <si>
@@ -692,32 +689,32 @@
     <t>https://www.digikey.ca/product-detail/en/qualtek/17-M100N-M/Q729-ND/4072231</t>
   </si>
   <si>
-    <t>Q729-ND</t>
-  </si>
-  <si>
-    <t>Qualtek</t>
-  </si>
-  <si>
     <t>36-4708-ND</t>
   </si>
   <si>
     <t>Keystone Electronics</t>
   </si>
   <si>
-    <t>17-M100N-M</t>
-  </si>
-  <si>
     <t>https://www.digikey.ca/product-detail/en/keystone-electronics/4708/36-4708-ND/4499301</t>
   </si>
   <si>
     <t>https://www.digikey.com/product-detail/en/keystone-electronics/4708/36-4708-ND/4499301</t>
+  </si>
+  <si>
+    <t>2-604771-9</t>
+  </si>
+  <si>
+    <t>TE Connectivity Raychem Cable Protection</t>
+  </si>
+  <si>
+    <t>2-604771-9-ND</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -859,6 +856,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="33">
@@ -1203,7 +1205,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -1211,6 +1213,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1569,8 +1572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D21" workbookViewId="0">
-      <selection activeCell="P31" sqref="P31"/>
+    <sheetView tabSelected="1" topLeftCell="D18" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1682,7 +1685,7 @@
         <v>145</v>
       </c>
       <c r="H3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>15</v>
@@ -1801,7 +1804,7 @@
         <v>24</v>
       </c>
       <c r="H7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>206</v>
@@ -1833,7 +1836,7 @@
         <v>146</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="O8" s="3" t="s">
         <v>38</v>
@@ -1865,7 +1868,7 @@
         <v>41</v>
       </c>
       <c r="H9" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>42</v>
@@ -1891,13 +1894,13 @@
         <v>34</v>
       </c>
       <c r="F10" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G10" t="s">
         <v>35</v>
       </c>
       <c r="H10" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="O10" s="1" t="s">
         <v>36</v>
@@ -2393,7 +2396,7 @@
         <v>92</v>
       </c>
       <c r="H27" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="O27" s="1" t="s">
         <v>191</v>
@@ -2425,7 +2428,7 @@
         <v>88</v>
       </c>
       <c r="H28" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="O28" s="1" t="s">
         <v>89</v>
@@ -2486,7 +2489,7 @@
         <v>167</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="O30" s="3" t="s">
         <v>169</v>
@@ -2509,19 +2512,19 @@
         <v>4708</v>
       </c>
       <c r="E31" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="F31" s="4">
         <v>4708</v>
       </c>
       <c r="G31" t="s">
+        <v>221</v>
+      </c>
+      <c r="O31" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="P31" s="1" t="s">
         <v>224</v>
-      </c>
-      <c r="O31" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="P31" s="1" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.2">
@@ -2576,7 +2579,7 @@
         <v>107</v>
       </c>
       <c r="H33" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="O33" s="1" t="s">
         <v>108</v>
@@ -2637,10 +2640,10 @@
         <v>125</v>
       </c>
       <c r="O35" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="P35" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.2">
@@ -2701,7 +2704,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>1</v>
       </c>
@@ -2712,25 +2715,22 @@
         <v>120</v>
       </c>
       <c r="D38" t="s">
+        <v>225</v>
+      </c>
+      <c r="E38" t="s">
         <v>226</v>
       </c>
-      <c r="E38" t="s">
-        <v>223</v>
-      </c>
       <c r="F38" t="s">
-        <v>226</v>
-      </c>
-      <c r="G38" t="s">
-        <v>222</v>
-      </c>
-      <c r="H38" t="s">
-        <v>208</v>
+        <v>225</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>227</v>
       </c>
       <c r="O38" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="P38" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Updated BOM file (March 12, 2018)
</commit_message>
<xml_diff>
--- a/LipSync_BOM.xlsx
+++ b/LipSync_BOM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="227">
   <si>
     <t>Qty</t>
   </si>
@@ -683,12 +683,6 @@
     <t>https://www.amazon.com/CAMVATE-Female-Male-Piece-Adapter/dp/B01GWVQ022</t>
   </si>
   <si>
-    <t>https://www.digikey.com/product-detail/en/qualtek/17-M100N-M/Q729-ND/4072231</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ca/product-detail/en/qualtek/17-M100N-M/Q729-ND/4072231</t>
-  </si>
-  <si>
     <t>36-4708-ND</t>
   </si>
   <si>
@@ -701,20 +695,23 @@
     <t>https://www.digikey.com/product-detail/en/keystone-electronics/4708/36-4708-ND/4499301</t>
   </si>
   <si>
-    <t>2-604771-9</t>
-  </si>
-  <si>
-    <t>TE Connectivity Raychem Cable Protection</t>
-  </si>
-  <si>
-    <t>2-604771-9-ND</t>
+    <t>Panduit Corp</t>
+  </si>
+  <si>
+    <t>298-1021-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/panduit-corp/PLT1M-M/298-1021-ND/280034</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/panduit-corp/PLT1M-M/298-1021-ND/280034</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -856,11 +853,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="33">
@@ -1205,7 +1197,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -1213,7 +1205,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1572,8 +1563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D18" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+    <sheetView tabSelected="1" topLeftCell="D17" workbookViewId="0">
+      <selection activeCell="P39" sqref="P39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2512,19 +2503,19 @@
         <v>4708</v>
       </c>
       <c r="E31" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F31" s="4">
         <v>4708</v>
       </c>
       <c r="G31" t="s">
+        <v>219</v>
+      </c>
+      <c r="O31" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="O31" s="1" t="s">
-        <v>223</v>
-      </c>
       <c r="P31" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.2">
@@ -2704,7 +2695,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="38" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>1</v>
       </c>
@@ -2715,22 +2706,22 @@
         <v>120</v>
       </c>
       <c r="D38" t="s">
+        <v>224</v>
+      </c>
+      <c r="E38" t="s">
+        <v>223</v>
+      </c>
+      <c r="F38" t="s">
+        <v>224</v>
+      </c>
+      <c r="G38" t="s">
+        <v>224</v>
+      </c>
+      <c r="O38" t="s">
         <v>225</v>
       </c>
-      <c r="E38" t="s">
+      <c r="P38" s="1" t="s">
         <v>226</v>
-      </c>
-      <c r="F38" t="s">
-        <v>225</v>
-      </c>
-      <c r="G38" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="O38" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="P38" s="1" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.2">
@@ -2898,7 +2889,7 @@
     <hyperlink ref="P40" r:id="rId74"/>
     <hyperlink ref="P41" r:id="rId75" display="http://www.digikey.ca/product-detail/en/sparkfun-electronics/WRL-12576/1568-1265-ND"/>
     <hyperlink ref="O36" r:id="rId76"/>
-    <hyperlink ref="O38" r:id="rId77"/>
+    <hyperlink ref="P38" r:id="rId77"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated BOM file (June 19, 2018)
</commit_message>
<xml_diff>
--- a/LipSync_BOM.xlsx
+++ b/LipSync_BOM.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="26215"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kmok/Documents/NSS/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kristina Mok\Dropbox\NSS\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{0ACD3C9D-0ECE-4CB0-B590-373341E7DE0D}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="13360"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8784" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LipSync_BOM" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="228">
   <si>
     <t>Qty</t>
   </si>
@@ -233,9 +234,6 @@
     <t>"11648"</t>
   </si>
   <si>
-    <t>http://www.qosina.com/male-luer-lock-stepped-connector-11648</t>
-  </si>
-  <si>
     <t xml:space="preserve">Filter PTFE Hydrophobic 17 mm, 0.2 Micron </t>
   </si>
   <si>
@@ -705,12 +703,18 @@
   </si>
   <si>
     <t>https://www.digikey.com/product-detail/en/panduit-corp/PLT1M-M/298-1021-ND/280034</t>
+  </si>
+  <si>
+    <t>https://www.qosina.com/stepped-male-luer-lock-connector-80102</t>
+  </si>
+  <si>
+    <t>"80102"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1560,32 +1564,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D17" workbookViewId="0">
-      <selection activeCell="P39" sqref="P39"/>
+    <sheetView tabSelected="1" topLeftCell="D11" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="50.5" customWidth="1"/>
-    <col min="4" max="4" width="35.5" customWidth="1"/>
-    <col min="6" max="6" width="24.83203125" customWidth="1"/>
+    <col min="3" max="3" width="50.44140625" customWidth="1"/>
+    <col min="4" max="4" width="35.44140625" customWidth="1"/>
+    <col min="6" max="6" width="24.77734375" customWidth="1"/>
     <col min="7" max="7" width="27.6640625" customWidth="1"/>
-    <col min="8" max="8" width="13.1640625" customWidth="1"/>
-    <col min="15" max="15" width="18.83203125" customWidth="1"/>
+    <col min="8" max="8" width="13.109375" customWidth="1"/>
+    <col min="15" max="15" width="18.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -1621,13 +1625,13 @@
         <v>4</v>
       </c>
       <c r="O1" t="s">
+        <v>177</v>
+      </c>
+      <c r="P1" t="s">
         <v>178</v>
       </c>
-      <c r="P1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="G2" t="s">
         <v>5</v>
       </c>
@@ -1653,15 +1657,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D3" t="s">
         <v>13</v>
@@ -1673,24 +1677,24 @@
         <v>13</v>
       </c>
       <c r="G3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>15</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C4" t="s">
         <v>25</v>
@@ -1711,73 +1715,73 @@
         <v>29</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C5" t="s">
         <v>30</v>
       </c>
       <c r="D5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E5" t="s">
         <v>31</v>
       </c>
       <c r="F5" t="s">
+        <v>132</v>
+      </c>
+      <c r="G5" t="s">
         <v>133</v>
       </c>
-      <c r="G5" t="s">
-        <v>134</v>
-      </c>
       <c r="O5" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C6" t="s">
+        <v>139</v>
+      </c>
+      <c r="D6" t="s">
         <v>140</v>
-      </c>
-      <c r="D6" t="s">
-        <v>141</v>
       </c>
       <c r="E6" t="s">
         <v>31</v>
       </c>
       <c r="F6" t="s">
+        <v>140</v>
+      </c>
+      <c r="G6" t="s">
         <v>141</v>
       </c>
-      <c r="G6" t="s">
+      <c r="O6" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="O6" s="1" t="s">
-        <v>143</v>
-      </c>
       <c r="P6" s="1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C7" t="s">
         <v>21</v>
@@ -1795,53 +1799,53 @@
         <v>24</v>
       </c>
       <c r="H7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="O7" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="P7" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="P7" s="1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>1</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>37</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>34</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="O8" s="3" t="s">
         <v>38</v>
       </c>
       <c r="P8" s="3" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C9" t="s">
         <v>39</v>
@@ -1859,21 +1863,21 @@
         <v>41</v>
       </c>
       <c r="H9" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>42</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C10" t="s">
         <v>32</v>
@@ -1885,27 +1889,27 @@
         <v>34</v>
       </c>
       <c r="F10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G10" t="s">
         <v>35</v>
       </c>
       <c r="H10" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="O10" s="1" t="s">
         <v>36</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C11" t="s">
         <v>58</v>
@@ -1926,73 +1930,73 @@
         <v>61</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>2</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="O12" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="O12" s="3" t="s">
-        <v>174</v>
-      </c>
       <c r="P12" s="3" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>2</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>155</v>
-      </c>
       <c r="F13" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="O13" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="P13" s="3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C14" t="s">
         <v>53</v>
@@ -2013,15 +2017,15 @@
         <v>57</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C15" t="s">
         <v>62</v>
@@ -2042,73 +2046,73 @@
         <v>65</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>1</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C16" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="E16" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="G16" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="O16" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="F16" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="O16" s="3" t="s">
-        <v>177</v>
-      </c>
       <c r="P16" s="3" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>1</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>66</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>55</v>
       </c>
       <c r="F17" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="O17" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="G17" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="O17" s="3" t="s">
-        <v>161</v>
-      </c>
       <c r="P17" s="3" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C18" t="s">
         <v>43</v>
@@ -2129,44 +2133,44 @@
         <v>47</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>1</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C19" t="s">
+        <v>134</v>
+      </c>
+      <c r="D19" t="s">
+        <v>136</v>
+      </c>
+      <c r="E19" t="s">
         <v>135</v>
       </c>
-      <c r="D19" t="s">
+      <c r="F19" t="s">
+        <v>136</v>
+      </c>
+      <c r="G19" t="s">
         <v>137</v>
       </c>
-      <c r="E19" t="s">
-        <v>136</v>
-      </c>
-      <c r="F19" t="s">
-        <v>137</v>
-      </c>
-      <c r="G19" t="s">
+      <c r="O19" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="O19" s="1" t="s">
-        <v>139</v>
-      </c>
       <c r="P19" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C20" t="s">
         <v>48</v>
@@ -2187,15 +2191,15 @@
         <v>52</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>1</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C21" t="s">
         <v>67</v>
@@ -2207,587 +2211,587 @@
         <v>7</v>
       </c>
       <c r="F21" t="s">
-        <v>68</v>
+        <v>227</v>
       </c>
       <c r="I21" t="s">
-        <v>68</v>
+        <v>227</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>69</v>
+        <v>226</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>1</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C22" t="s">
+        <v>69</v>
+      </c>
+      <c r="D22" t="s">
         <v>70</v>
-      </c>
-      <c r="D22" t="s">
-        <v>71</v>
       </c>
       <c r="E22" t="s">
         <v>7</v>
       </c>
       <c r="F22" t="s">
+        <v>70</v>
+      </c>
+      <c r="I22" t="s">
+        <v>70</v>
+      </c>
+      <c r="O22" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="I22" t="s">
+      <c r="P22" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="O22" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="P22" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>1</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C23" t="s">
+        <v>72</v>
+      </c>
+      <c r="D23" t="s">
         <v>73</v>
-      </c>
-      <c r="D23" t="s">
-        <v>74</v>
       </c>
       <c r="E23" t="s">
         <v>8</v>
       </c>
       <c r="F23" t="s">
+        <v>73</v>
+      </c>
+      <c r="J23" t="s">
+        <v>73</v>
+      </c>
+      <c r="O23" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="J23" t="s">
+      <c r="P23" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="O23" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="P23" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>4</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C24" t="s">
+        <v>75</v>
+      </c>
+      <c r="D24" t="s">
         <v>76</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>77</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
+        <v>76</v>
+      </c>
+      <c r="G24" t="s">
         <v>78</v>
       </c>
-      <c r="F24" t="s">
-        <v>77</v>
-      </c>
-      <c r="G24" t="s">
+      <c r="O24" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="P24" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="O24" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="P24" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>4</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C25" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G25" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="D25" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="E25" s="2" t="s">
+      <c r="O25" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="F25" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="O25" s="3" t="s">
-        <v>166</v>
-      </c>
       <c r="P25" s="3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>6</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C26" t="s">
+        <v>80</v>
+      </c>
+      <c r="D26" t="s">
         <v>81</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>82</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
+        <v>81</v>
+      </c>
+      <c r="K26" t="s">
+        <v>81</v>
+      </c>
+      <c r="O26" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="F26" t="s">
-        <v>82</v>
-      </c>
-      <c r="K26" t="s">
-        <v>82</v>
-      </c>
-      <c r="O26" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="P26" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>2</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C27" t="s">
+        <v>89</v>
+      </c>
+      <c r="D27" t="s">
         <v>90</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
+        <v>86</v>
+      </c>
+      <c r="F27" t="s">
+        <v>90</v>
+      </c>
+      <c r="G27" t="s">
         <v>91</v>
       </c>
-      <c r="E27" t="s">
-        <v>87</v>
-      </c>
-      <c r="F27" t="s">
-        <v>91</v>
-      </c>
-      <c r="G27" t="s">
+      <c r="H27" t="s">
+        <v>212</v>
+      </c>
+      <c r="O27" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="P27" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="H27" t="s">
-        <v>213</v>
-      </c>
-      <c r="O27" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="P27" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>2</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C28" t="s">
+        <v>84</v>
+      </c>
+      <c r="D28" t="s">
         <v>85</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>86</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
+        <v>85</v>
+      </c>
+      <c r="G28" t="s">
         <v>87</v>
       </c>
-      <c r="F28" t="s">
-        <v>86</v>
-      </c>
-      <c r="G28" t="s">
+      <c r="H28" t="s">
+        <v>213</v>
+      </c>
+      <c r="O28" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="H28" t="s">
-        <v>214</v>
-      </c>
-      <c r="O28" s="1" t="s">
-        <v>89</v>
-      </c>
       <c r="P28" s="1" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>1</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C29" t="s">
+        <v>93</v>
+      </c>
+      <c r="D29" t="s">
         <v>94</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>95</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
+        <v>94</v>
+      </c>
+      <c r="J29" t="s">
+        <v>94</v>
+      </c>
+      <c r="O29" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="F29" t="s">
-        <v>95</v>
-      </c>
-      <c r="J29" t="s">
-        <v>95</v>
-      </c>
-      <c r="O29" s="1" t="s">
-        <v>97</v>
-      </c>
       <c r="P29" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>4</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>50</v>
       </c>
       <c r="F30" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="O30" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="G30" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="O30" s="3" t="s">
-        <v>169</v>
-      </c>
       <c r="P30" s="3" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>4</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C31" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D31" s="4">
         <v>4708</v>
       </c>
       <c r="E31" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F31" s="4">
         <v>4708</v>
       </c>
       <c r="G31" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="O31" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="P31" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="P31" s="1" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>1</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C32" t="s">
+        <v>99</v>
+      </c>
+      <c r="D32" t="s">
         <v>100</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>101</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32" t="s">
+        <v>100</v>
+      </c>
+      <c r="L32" t="s">
+        <v>100</v>
+      </c>
+      <c r="O32" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="F32" t="s">
-        <v>101</v>
-      </c>
-      <c r="L32" t="s">
-        <v>101</v>
-      </c>
-      <c r="O32" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="P32" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>1</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C33" t="s">
+        <v>103</v>
+      </c>
+      <c r="D33" t="s">
         <v>104</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
         <v>105</v>
       </c>
-      <c r="E33" t="s">
+      <c r="F33" t="s">
+        <v>104</v>
+      </c>
+      <c r="G33" t="s">
         <v>106</v>
       </c>
-      <c r="F33" t="s">
-        <v>105</v>
-      </c>
-      <c r="G33" t="s">
+      <c r="H33" t="s">
+        <v>215</v>
+      </c>
+      <c r="O33" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="H33" t="s">
-        <v>216</v>
-      </c>
-      <c r="O33" s="1" t="s">
-        <v>108</v>
-      </c>
       <c r="P33" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>1</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C34" t="s">
+        <v>108</v>
+      </c>
+      <c r="D34" t="s">
         <v>109</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E34" t="s">
         <v>110</v>
       </c>
-      <c r="E34" t="s">
+      <c r="F34" t="s">
+        <v>109</v>
+      </c>
+      <c r="M34" t="s">
         <v>111</v>
       </c>
-      <c r="F34" t="s">
-        <v>110</v>
-      </c>
-      <c r="M34" t="s">
+      <c r="O34" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="O34" s="1" t="s">
-        <v>113</v>
-      </c>
       <c r="P34" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>1</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C35" t="s">
+        <v>123</v>
+      </c>
+      <c r="D35" t="s">
         <v>124</v>
       </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
         <v>125</v>
       </c>
-      <c r="E35" t="s">
-        <v>126</v>
-      </c>
       <c r="F35" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="N35" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="O35" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="P35" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>1</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C36" t="s">
+        <v>113</v>
+      </c>
+      <c r="D36" t="s">
         <v>114</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E36" t="s">
         <v>115</v>
       </c>
-      <c r="E36" t="s">
-        <v>116</v>
-      </c>
       <c r="F36" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="N36" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="O36" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="P36" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>1</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C37" t="s">
+        <v>116</v>
+      </c>
+      <c r="D37" t="s">
+        <v>116</v>
+      </c>
+      <c r="E37" t="s">
         <v>117</v>
       </c>
-      <c r="D37" t="s">
-        <v>117</v>
-      </c>
-      <c r="E37" t="s">
+      <c r="F37" t="s">
+        <v>116</v>
+      </c>
+      <c r="N37" t="s">
         <v>118</v>
       </c>
-      <c r="F37" t="s">
-        <v>117</v>
-      </c>
-      <c r="N37" t="s">
-        <v>119</v>
-      </c>
       <c r="O37" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="P37" s="1" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>1</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C38" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D38" t="s">
+        <v>223</v>
+      </c>
+      <c r="E38" t="s">
+        <v>222</v>
+      </c>
+      <c r="F38" t="s">
+        <v>223</v>
+      </c>
+      <c r="G38" t="s">
+        <v>223</v>
+      </c>
+      <c r="O38" t="s">
         <v>224</v>
       </c>
-      <c r="E38" t="s">
-        <v>223</v>
-      </c>
-      <c r="F38" t="s">
-        <v>224</v>
-      </c>
-      <c r="G38" t="s">
-        <v>224</v>
-      </c>
-      <c r="O38" t="s">
+      <c r="P38" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="P38" s="1" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>10</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C39" t="s">
+        <v>126</v>
+      </c>
+      <c r="D39" t="s">
         <v>127</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
         <v>128</v>
       </c>
-      <c r="E39" t="s">
+      <c r="F39" t="s">
+        <v>127</v>
+      </c>
+      <c r="M39" t="s">
         <v>129</v>
       </c>
-      <c r="F39" t="s">
-        <v>128</v>
-      </c>
-      <c r="M39" t="s">
+      <c r="O39" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="O39" s="1" t="s">
-        <v>131</v>
-      </c>
       <c r="P39" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>1</v>
       </c>
       <c r="B40" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C40" t="s">
+        <v>120</v>
+      </c>
+      <c r="D40" t="s">
         <v>121</v>
       </c>
-      <c r="D40" t="s">
+      <c r="E40" t="s">
         <v>122</v>
       </c>
-      <c r="E40" t="s">
-        <v>123</v>
-      </c>
       <c r="F40" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="N40" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="O40" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="P40" s="1" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>1</v>
       </c>
       <c r="B41" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C41" t="s">
         <v>16</v>
@@ -2808,88 +2812,86 @@
         <v>20</v>
       </c>
       <c r="P41" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="O5" r:id="rId1"/>
-    <hyperlink ref="O7" r:id="rId2"/>
-    <hyperlink ref="O41" r:id="rId3"/>
-    <hyperlink ref="O6" r:id="rId4"/>
-    <hyperlink ref="O19" r:id="rId5"/>
-    <hyperlink ref="O10" r:id="rId6"/>
-    <hyperlink ref="O8" r:id="rId7"/>
-    <hyperlink ref="O9" r:id="rId8"/>
-    <hyperlink ref="O18" r:id="rId9"/>
-    <hyperlink ref="O20" r:id="rId10"/>
-    <hyperlink ref="O14" r:id="rId11"/>
-    <hyperlink ref="O12" r:id="rId12"/>
-    <hyperlink ref="O11" r:id="rId13"/>
-    <hyperlink ref="O15" r:id="rId14"/>
-    <hyperlink ref="O16" r:id="rId15"/>
-    <hyperlink ref="O17" r:id="rId16"/>
-    <hyperlink ref="O21" r:id="rId17"/>
-    <hyperlink ref="O22" r:id="rId18"/>
-    <hyperlink ref="O23" r:id="rId19"/>
-    <hyperlink ref="O24" r:id="rId20"/>
-    <hyperlink ref="O25" r:id="rId21"/>
-    <hyperlink ref="O26" r:id="rId22"/>
-    <hyperlink ref="O28" r:id="rId23"/>
-    <hyperlink ref="O27" r:id="rId24"/>
-    <hyperlink ref="O29" r:id="rId25"/>
-    <hyperlink ref="O30" r:id="rId26"/>
-    <hyperlink ref="O31" r:id="rId27"/>
-    <hyperlink ref="O32" r:id="rId28"/>
-    <hyperlink ref="O33" r:id="rId29"/>
-    <hyperlink ref="O34" r:id="rId30"/>
-    <hyperlink ref="O37" r:id="rId31"/>
-    <hyperlink ref="O40" r:id="rId32"/>
-    <hyperlink ref="O35" r:id="rId33"/>
-    <hyperlink ref="O39" r:id="rId34"/>
-    <hyperlink ref="O3" r:id="rId35"/>
-    <hyperlink ref="O4" r:id="rId36"/>
-    <hyperlink ref="O13" r:id="rId37"/>
-    <hyperlink ref="P3" r:id="rId38"/>
-    <hyperlink ref="P4" r:id="rId39"/>
-    <hyperlink ref="P5" r:id="rId40"/>
-    <hyperlink ref="P6" r:id="rId41"/>
-    <hyperlink ref="P7" r:id="rId42"/>
-    <hyperlink ref="P8" r:id="rId43"/>
-    <hyperlink ref="P9" r:id="rId44"/>
-    <hyperlink ref="P10" r:id="rId45"/>
-    <hyperlink ref="P11" r:id="rId46"/>
-    <hyperlink ref="P12" r:id="rId47" display="https://www.digikey.ca/product-detail/en/molex-connector-corporation/22-05-2031/WM4101-ND/"/>
-    <hyperlink ref="P13" r:id="rId48" display="https://www.digikey.ca/product-detail/en/preci-dip/801-87-003-10-001101/1212-1180-ND"/>
-    <hyperlink ref="P14" r:id="rId49"/>
-    <hyperlink ref="P15" r:id="rId50"/>
-    <hyperlink ref="P16" r:id="rId51" display="https://www.digikey.ca/product-detail/en/everlight-electronics-co-ltd/MV5437/1080-1109-ND/2675600"/>
-    <hyperlink ref="P17" r:id="rId52" display="https://www.digikey.ca/product-detail/en/sullins-connector-solutions/SPC02SYAN/S9002-ND"/>
-    <hyperlink ref="P18" r:id="rId53" display="http://www.digikey.ca/product-detail/en/fairchild-on-semiconductor/2N3906TFR/2N3906D26ZCT-ND"/>
-    <hyperlink ref="P19" r:id="rId54" display="https://www.digikey.ca/product-detail/en/sullins-connector-solutions/PPPC061LFBN-RC/S7039-ND"/>
-    <hyperlink ref="P20" r:id="rId55" display="http://www.digikey.ca/product-detail/en/3m/929974-01-01/929974-01-01-ND"/>
-    <hyperlink ref="P21" r:id="rId56"/>
-    <hyperlink ref="P22" r:id="rId57"/>
-    <hyperlink ref="P23" r:id="rId58"/>
-    <hyperlink ref="P24" r:id="rId59"/>
-    <hyperlink ref="P25" r:id="rId60" display="https://www.digikey.ca/product-detail/en/essentra-components/NMS-308/RP809-ND"/>
-    <hyperlink ref="P26" r:id="rId61"/>
-    <hyperlink ref="P27" r:id="rId62"/>
-    <hyperlink ref="P28" r:id="rId63" display="http://www.digikey.ca/product-detail/en/keystone-electronics/25503/36-25503-ND/"/>
-    <hyperlink ref="P29" r:id="rId64"/>
-    <hyperlink ref="P30" r:id="rId65" display="https://www.digikey.ca/product-detail/en/3m/SJ-5003-(BLACK)/SJ5003-0-ND/102573"/>
-    <hyperlink ref="P31" r:id="rId66"/>
-    <hyperlink ref="P32" r:id="rId67"/>
-    <hyperlink ref="P33" r:id="rId68"/>
-    <hyperlink ref="P34" r:id="rId69"/>
-    <hyperlink ref="P35" r:id="rId70"/>
-    <hyperlink ref="P36" r:id="rId71"/>
-    <hyperlink ref="P37" r:id="rId72"/>
-    <hyperlink ref="P39" r:id="rId73"/>
-    <hyperlink ref="P40" r:id="rId74"/>
-    <hyperlink ref="P41" r:id="rId75" display="http://www.digikey.ca/product-detail/en/sparkfun-electronics/WRL-12576/1568-1265-ND"/>
-    <hyperlink ref="O36" r:id="rId76"/>
-    <hyperlink ref="P38" r:id="rId77"/>
+    <hyperlink ref="O5" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="O7" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="O41" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="O6" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="O19" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="O10" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="O8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="O9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="O18" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="O20" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="O14" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="O12" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="O11" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="O15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="O16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="O17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="O22" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="O23" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="O24" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="O25" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="O26" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="O28" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="O27" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="O29" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="O30" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="O31" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="O32" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="O33" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="O34" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="O37" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="O40" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="O35" r:id="rId32" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="O39" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="O3" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="O4" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="O13" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="P3" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="P4" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="P5" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="P6" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="P7" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="P8" r:id="rId42" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="P9" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="P10" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="P11" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="P12" r:id="rId46" display="https://www.digikey.ca/product-detail/en/molex-connector-corporation/22-05-2031/WM4101-ND/" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="P13" r:id="rId47" display="https://www.digikey.ca/product-detail/en/preci-dip/801-87-003-10-001101/1212-1180-ND" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="P14" r:id="rId48" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="P15" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="P16" r:id="rId50" display="https://www.digikey.ca/product-detail/en/everlight-electronics-co-ltd/MV5437/1080-1109-ND/2675600" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="P17" r:id="rId51" display="https://www.digikey.ca/product-detail/en/sullins-connector-solutions/SPC02SYAN/S9002-ND" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="P18" r:id="rId52" display="http://www.digikey.ca/product-detail/en/fairchild-on-semiconductor/2N3906TFR/2N3906D26ZCT-ND" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="P19" r:id="rId53" display="https://www.digikey.ca/product-detail/en/sullins-connector-solutions/PPPC061LFBN-RC/S7039-ND" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="P20" r:id="rId54" display="http://www.digikey.ca/product-detail/en/3m/929974-01-01/929974-01-01-ND" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="P22" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="P23" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="P24" r:id="rId57" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="P25" r:id="rId58" display="https://www.digikey.ca/product-detail/en/essentra-components/NMS-308/RP809-ND" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="P26" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="P27" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="P28" r:id="rId61" display="http://www.digikey.ca/product-detail/en/keystone-electronics/25503/36-25503-ND/" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="P29" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="P30" r:id="rId63" display="https://www.digikey.ca/product-detail/en/3m/SJ-5003-(BLACK)/SJ5003-0-ND/102573" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="P31" r:id="rId64" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="P32" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="P33" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="P34" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="P35" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="P36" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="P37" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="P39" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="P40" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="P41" r:id="rId73" display="http://www.digikey.ca/product-detail/en/sparkfun-electronics/WRL-12576/1568-1265-ND" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="O36" r:id="rId74" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="P38" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated BOM file (July 3, 2018)
</commit_message>
<xml_diff>
--- a/LipSync_BOM.xlsx
+++ b/LipSync_BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kristina Mok\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{CE70BEC2-19C7-4CFE-BF8A-CBD17CEB0FFF}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{A8A077B6-9E73-40E9-BDB2-DDCE9645ED90}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8784" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="232">
   <si>
     <t>Qty</t>
   </si>
@@ -531,9 +531,6 @@
     <t xml:space="preserve">SJ-5003 (BLACK) </t>
   </si>
   <si>
-    <t>https://www.digikey.ca/product-detail/en/3m/SJ-5003-(BLACK)/SJ5003-0-ND/102573</t>
-  </si>
-  <si>
     <t>Component name (October 25,2017)</t>
   </si>
   <si>
@@ -702,16 +699,28 @@
     <t>"80102"</t>
   </si>
   <si>
-    <t>https://www.digikey.ca/product-detail/en/te-connectivity-raychem-cable-protection/2-604771-9/2-604771-9-ND/2259327</t>
-  </si>
-  <si>
     <t>2-604771-9-ND</t>
   </si>
   <si>
     <t xml:space="preserve">2-604771-9 </t>
   </si>
   <si>
-    <t>https://www.digikey.com/product-detail/en/te-connectivity-raychem-cable-protection/2-604771-9/2-604771-9-ND/2259327</t>
+    <t>https://www.mouser.ca/ProductDetail/3M-Electronic-Specialty/SJ-5003-BLACK?qs=sGAEpiMZZMvlOED0T0kTWubpGv7E7tyx</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Panduit/PLT6SM-M?qs=sGAEpiMZZMv3%2fYgcm0iDLApe1nFw7TiN%2fRMgiNKPBi8%3d</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Panduit/PLT6SM-M?qs=sGAEpiMZZMv3%2fYgcm0iDLApe1nFw7TiN%2fRMgiNKPBi8=</t>
+  </si>
+  <si>
+    <t xml:space="preserve">644-PLT.6SM-M </t>
+  </si>
+  <si>
+    <t>https://www.adorama.com/wtm11.html</t>
+  </si>
+  <si>
+    <t>https://www.amazon.ca/Wpeng-Female-degree-Micro-Splitter/dp/B01M5F47SY/ref=sr_1_2?ie=UTF8&amp;qid=1530643192&amp;sr=8-2&amp;keywords=Micro+USB+Male+To+USB+Female+Host+OTG+Cable+%2B+USB+Power+Cable+Y+Splitter</t>
   </si>
 </sst>
 </file>
@@ -1576,8 +1585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D29" workbookViewId="0">
-      <selection activeCell="P38" sqref="O38:P38"/>
+    <sheetView tabSelected="1" topLeftCell="D20" workbookViewId="0">
+      <selection activeCell="O37" sqref="O37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1595,10 +1604,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -1634,10 +1643,10 @@
         <v>4</v>
       </c>
       <c r="O1" t="s">
+        <v>176</v>
+      </c>
+      <c r="P1" t="s">
         <v>177</v>
-      </c>
-      <c r="P1" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
@@ -1671,7 +1680,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C3" t="s">
         <v>143</v>
@@ -1689,13 +1698,13 @@
         <v>144</v>
       </c>
       <c r="H3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>15</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
@@ -1703,7 +1712,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C4" t="s">
         <v>25</v>
@@ -1724,7 +1733,7 @@
         <v>29</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
@@ -1732,7 +1741,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C5" t="s">
         <v>30</v>
@@ -1753,7 +1762,7 @@
         <v>131</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
@@ -1761,7 +1770,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C6" t="s">
         <v>139</v>
@@ -1782,7 +1791,7 @@
         <v>142</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
@@ -1790,7 +1799,7 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C7" t="s">
         <v>21</v>
@@ -1808,13 +1817,13 @@
         <v>24</v>
       </c>
       <c r="H7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="O7" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="P7" s="1" t="s">
         <v>205</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -1822,7 +1831,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>37</v>
@@ -1840,13 +1849,13 @@
         <v>145</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="O8" s="3" t="s">
         <v>38</v>
       </c>
       <c r="P8" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
@@ -1854,7 +1863,7 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C9" t="s">
         <v>39</v>
@@ -1872,13 +1881,13 @@
         <v>41</v>
       </c>
       <c r="H9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>42</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
@@ -1886,7 +1895,7 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C10" t="s">
         <v>32</v>
@@ -1898,19 +1907,19 @@
         <v>34</v>
       </c>
       <c r="F10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G10" t="s">
         <v>35</v>
       </c>
       <c r="H10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="O10" s="1" t="s">
         <v>36</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
@@ -1918,7 +1927,7 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C11" t="s">
         <v>58</v>
@@ -1939,7 +1948,7 @@
         <v>61</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -1947,7 +1956,7 @@
         <v>2</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>149</v>
@@ -1965,10 +1974,10 @@
         <v>150</v>
       </c>
       <c r="O12" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="P12" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -1976,7 +1985,7 @@
         <v>2</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>153</v>
@@ -1994,10 +2003,10 @@
         <v>147</v>
       </c>
       <c r="O13" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="P13" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
@@ -2005,7 +2014,7 @@
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C14" t="s">
         <v>53</v>
@@ -2026,7 +2035,7 @@
         <v>57</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
@@ -2034,7 +2043,7 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C15" t="s">
         <v>62</v>
@@ -2055,7 +2064,7 @@
         <v>65</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -2063,7 +2072,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>155</v>
@@ -2072,7 +2081,7 @@
         <v>156</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>156</v>
@@ -2081,10 +2090,10 @@
         <v>157</v>
       </c>
       <c r="O16" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="P16" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -2092,7 +2101,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>66</v>
@@ -2113,7 +2122,7 @@
         <v>160</v>
       </c>
       <c r="P17" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.3">
@@ -2121,7 +2130,7 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C18" t="s">
         <v>43</v>
@@ -2142,7 +2151,7 @@
         <v>47</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.3">
@@ -2150,7 +2159,7 @@
         <v>1</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C19" t="s">
         <v>134</v>
@@ -2171,7 +2180,7 @@
         <v>138</v>
       </c>
       <c r="P19" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.3">
@@ -2179,7 +2188,7 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C20" t="s">
         <v>48</v>
@@ -2200,7 +2209,7 @@
         <v>52</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.3">
@@ -2208,7 +2217,7 @@
         <v>1</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C21" t="s">
         <v>67</v>
@@ -2220,16 +2229,16 @@
         <v>7</v>
       </c>
       <c r="F21" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I21" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.3">
@@ -2237,7 +2246,7 @@
         <v>1</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C22" t="s">
         <v>69</v>
@@ -2266,7 +2275,7 @@
         <v>1</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C23" t="s">
         <v>72</v>
@@ -2295,7 +2304,7 @@
         <v>4</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C24" t="s">
         <v>75</v>
@@ -2313,7 +2322,7 @@
         <v>78</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="P24" s="1" t="s">
         <v>79</v>
@@ -2324,7 +2333,7 @@
         <v>4</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>161</v>
@@ -2345,7 +2354,7 @@
         <v>165</v>
       </c>
       <c r="P25" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.3">
@@ -2353,7 +2362,7 @@
         <v>6</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C26" t="s">
         <v>80</v>
@@ -2382,7 +2391,7 @@
         <v>2</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C27" t="s">
         <v>89</v>
@@ -2400,10 +2409,10 @@
         <v>91</v>
       </c>
       <c r="H27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="P27" s="1" t="s">
         <v>92</v>
@@ -2414,7 +2423,7 @@
         <v>2</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C28" t="s">
         <v>84</v>
@@ -2432,13 +2441,13 @@
         <v>87</v>
       </c>
       <c r="H28" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="O28" s="1" t="s">
         <v>88</v>
       </c>
       <c r="P28" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.3">
@@ -2446,7 +2455,7 @@
         <v>1</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C29" t="s">
         <v>93</v>
@@ -2475,7 +2484,7 @@
         <v>4</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>97</v>
@@ -2493,13 +2502,13 @@
         <v>166</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="O30" s="3" t="s">
-        <v>168</v>
+        <v>226</v>
       </c>
       <c r="P30" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.3">
@@ -2507,7 +2516,7 @@
         <v>4</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C31" t="s">
         <v>98</v>
@@ -2516,19 +2525,19 @@
         <v>4708</v>
       </c>
       <c r="E31" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F31" s="4">
         <v>4708</v>
       </c>
       <c r="G31" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="O31" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="P31" s="1" t="s">
         <v>220</v>
-      </c>
-      <c r="P31" s="1" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.3">
@@ -2536,7 +2545,7 @@
         <v>1</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C32" t="s">
         <v>99</v>
@@ -2565,7 +2574,7 @@
         <v>1</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C33" t="s">
         <v>103</v>
@@ -2583,7 +2592,7 @@
         <v>106</v>
       </c>
       <c r="H33" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="O33" s="1" t="s">
         <v>107</v>
@@ -2597,7 +2606,7 @@
         <v>1</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C34" t="s">
         <v>108</v>
@@ -2618,7 +2627,7 @@
         <v>112</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>112</v>
+        <v>230</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.3">
@@ -2626,7 +2635,7 @@
         <v>1</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C35" t="s">
         <v>123</v>
@@ -2644,10 +2653,10 @@
         <v>124</v>
       </c>
       <c r="O35" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="P35" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.3">
@@ -2655,7 +2664,7 @@
         <v>1</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C36" t="s">
         <v>113</v>
@@ -2673,10 +2682,10 @@
         <v>113</v>
       </c>
       <c r="O36" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="P36" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="37" spans="1:16" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -2684,7 +2693,7 @@
         <v>1</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C37" t="s">
         <v>116</v>
@@ -2702,10 +2711,10 @@
         <v>118</v>
       </c>
       <c r="O37" s="1" t="s">
-        <v>192</v>
+        <v>231</v>
       </c>
       <c r="P37" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.3">
@@ -2713,28 +2722,31 @@
         <v>1</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C38" t="s">
         <v>119</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E38" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F38" t="s">
+        <v>225</v>
+      </c>
+      <c r="G38" t="s">
+        <v>229</v>
+      </c>
+      <c r="H38" t="s">
+        <v>229</v>
+      </c>
+      <c r="O38" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="P38" s="1" t="s">
         <v>227</v>
-      </c>
-      <c r="G38" s="6" t="s">
-        <v>226</v>
-      </c>
-      <c r="O38" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="P38" s="1" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.3">
@@ -2742,7 +2754,7 @@
         <v>10</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C39" t="s">
         <v>126</v>
@@ -2771,7 +2783,7 @@
         <v>1</v>
       </c>
       <c r="B40" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C40" t="s">
         <v>120</v>
@@ -2789,10 +2801,10 @@
         <v>120</v>
       </c>
       <c r="O40" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="P40" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.3">
@@ -2800,7 +2812,7 @@
         <v>1</v>
       </c>
       <c r="B41" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C41" t="s">
         <v>16</v>
@@ -2821,7 +2833,7 @@
         <v>20</v>
       </c>
       <c r="P41" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.3">
@@ -2853,58 +2865,53 @@
     <hyperlink ref="O28" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
     <hyperlink ref="O27" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
     <hyperlink ref="O29" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="O30" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="O31" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="O32" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="O33" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="O34" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="O37" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="O40" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="O35" r:id="rId32" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="O39" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="O3" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="O4" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="O13" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="P3" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="P4" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="P5" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="P6" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="P7" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="P8" r:id="rId42" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="P9" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="P10" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="P11" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="P12" r:id="rId46" display="https://www.digikey.ca/product-detail/en/molex-connector-corporation/22-05-2031/WM4101-ND/" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="P13" r:id="rId47" display="https://www.digikey.ca/product-detail/en/preci-dip/801-87-003-10-001101/1212-1180-ND" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="P14" r:id="rId48" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink ref="P15" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="P16" r:id="rId50" display="https://www.digikey.ca/product-detail/en/everlight-electronics-co-ltd/MV5437/1080-1109-ND/2675600" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="P17" r:id="rId51" display="https://www.digikey.ca/product-detail/en/sullins-connector-solutions/SPC02SYAN/S9002-ND" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink ref="P18" r:id="rId52" display="http://www.digikey.ca/product-detail/en/fairchild-on-semiconductor/2N3906TFR/2N3906D26ZCT-ND" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="P19" r:id="rId53" display="https://www.digikey.ca/product-detail/en/sullins-connector-solutions/PPPC061LFBN-RC/S7039-ND" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="P20" r:id="rId54" display="http://www.digikey.ca/product-detail/en/3m/929974-01-01/929974-01-01-ND" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink ref="P22" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink ref="P23" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink ref="P24" r:id="rId57" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
-    <hyperlink ref="P25" r:id="rId58" display="https://www.digikey.ca/product-detail/en/essentra-components/NMS-308/RP809-ND" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink ref="P26" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="P27" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
-    <hyperlink ref="P28" r:id="rId61" display="http://www.digikey.ca/product-detail/en/keystone-electronics/25503/36-25503-ND/" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
-    <hyperlink ref="P29" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
-    <hyperlink ref="P30" r:id="rId63" display="https://www.digikey.ca/product-detail/en/3m/SJ-5003-(BLACK)/SJ5003-0-ND/102573" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
-    <hyperlink ref="P31" r:id="rId64" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink ref="P32" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
-    <hyperlink ref="P33" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
-    <hyperlink ref="P34" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
-    <hyperlink ref="P35" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
-    <hyperlink ref="P36" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
-    <hyperlink ref="P37" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
-    <hyperlink ref="P39" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
-    <hyperlink ref="P40" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
-    <hyperlink ref="P41" r:id="rId73" display="http://www.digikey.ca/product-detail/en/sparkfun-electronics/WRL-12576/1568-1265-ND" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
-    <hyperlink ref="O36" r:id="rId74" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
-    <hyperlink ref="P38" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
-    <hyperlink ref="O38" r:id="rId76" xr:uid="{4BB3F8B2-09D0-4462-9D4D-E6544465F128}"/>
+    <hyperlink ref="O31" r:id="rId25" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="O32" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="O33" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="O34" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="O40" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="O35" r:id="rId30" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="O39" r:id="rId31" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="O3" r:id="rId32" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="O4" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="O13" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="P3" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="P4" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="P5" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="P6" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="P7" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="P8" r:id="rId40" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="P9" r:id="rId41" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="P10" r:id="rId42" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="P11" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="P12" r:id="rId44" display="https://www.digikey.ca/product-detail/en/molex-connector-corporation/22-05-2031/WM4101-ND/" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="P13" r:id="rId45" display="https://www.digikey.ca/product-detail/en/preci-dip/801-87-003-10-001101/1212-1180-ND" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="P14" r:id="rId46" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="P15" r:id="rId47" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="P16" r:id="rId48" display="https://www.digikey.ca/product-detail/en/everlight-electronics-co-ltd/MV5437/1080-1109-ND/2675600" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="P17" r:id="rId49" display="https://www.digikey.ca/product-detail/en/sullins-connector-solutions/SPC02SYAN/S9002-ND" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="P18" r:id="rId50" display="http://www.digikey.ca/product-detail/en/fairchild-on-semiconductor/2N3906TFR/2N3906D26ZCT-ND" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="P19" r:id="rId51" display="https://www.digikey.ca/product-detail/en/sullins-connector-solutions/PPPC061LFBN-RC/S7039-ND" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="P20" r:id="rId52" display="http://www.digikey.ca/product-detail/en/3m/929974-01-01/929974-01-01-ND" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="P22" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="P23" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="P24" r:id="rId55" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="P25" r:id="rId56" display="https://www.digikey.ca/product-detail/en/essentra-components/NMS-308/RP809-ND" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="P26" r:id="rId57" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="P27" r:id="rId58" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="P28" r:id="rId59" display="http://www.digikey.ca/product-detail/en/keystone-electronics/25503/36-25503-ND/" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="P29" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="P30" r:id="rId61" display="https://www.digikey.ca/product-detail/en/3m/SJ-5003-(BLACK)/SJ5003-0-ND/102573" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="P31" r:id="rId62" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="P32" r:id="rId63" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="P33" r:id="rId64" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="P35" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="P36" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="P37" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="P39" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="P40" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="P41" r:id="rId70" display="http://www.digikey.ca/product-detail/en/sparkfun-electronics/WRL-12576/1568-1265-ND" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="O36" r:id="rId71" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added the updated LipSync Manual, LipSync User Guide, LipSync Startup Guide, and LipSync BOM File.
</commit_message>
<xml_diff>
--- a/LipSync_BOM.xlsx
+++ b/LipSync_BOM.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Milad\Dropbox\Makers Making Change\Projects\LipSync\Github\LipSync\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kristina Mok\Dropbox\NSS\Downloads\LipSync Files\Mouse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87D2CCA1-6A09-44EB-ABEB-50B6EDDD5FDE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2B5E77A-991D-411D-9618-E69EC241887B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="20700" windowHeight="11140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="1770" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LipSync_BOM" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="228">
   <si>
     <t>Qty</t>
   </si>
@@ -156,21 +156,9 @@
     <t>http://www.digikey.ca/product-detail/en/fairchild-on-semiconductor/2N3906TFR/2N3906D26ZCT-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">1-Position Straight Female Through-Hole Header </t>
-  </si>
-  <si>
-    <t>929974-01-01</t>
-  </si>
-  <si>
     <t>3M</t>
   </si>
   <si>
-    <t>929974-01-01-ND</t>
-  </si>
-  <si>
-    <t>http://www.digikey.ca/product-detail/en/3m/929974-01-01/929974-01-01-ND</t>
-  </si>
-  <si>
     <t xml:space="preserve">4-Position Straight Female Through-Hole Header  </t>
   </si>
   <si>
@@ -387,21 +375,6 @@
     <t xml:space="preserve">CAMVATE </t>
   </si>
   <si>
-    <t xml:space="preserve">Velcro Cable Tie </t>
-  </si>
-  <si>
-    <t>S0506-10-B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pearstone </t>
-  </si>
-  <si>
-    <t xml:space="preserve">PES050610B </t>
-  </si>
-  <si>
-    <t>https://www.bhphotovideo.com/c/product/733008-REG/Pearstone_s0506_10_b_5_x_6_Touch.html</t>
-  </si>
-  <si>
     <t>https://www.digikey.ca/product-detail/en/stackpole-electronics-inc/CF14JT300R/CF14JT300RCT-ND</t>
   </si>
   <si>
@@ -604,9 +577,6 @@
   </si>
   <si>
     <t>http://www.digikey.com/product-detail/en/fairchild-on-semiconductor/2N3906TFR/2N3906D26ZCT-ND</t>
-  </si>
-  <si>
-    <t>http://www.digikey.com/product-detail/en/3m/929974-01-01/929974-01-01-ND</t>
   </si>
   <si>
     <t>http://www.digikey.com/product-detail/en/keystone-electronics/25503/36-25503-ND/</t>
@@ -1597,34 +1567,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41:XFD41"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39:XFD40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="50.453125" customWidth="1"/>
-    <col min="4" max="4" width="35.453125" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="23.08984375" customWidth="1"/>
-    <col min="6" max="6" width="16.6328125" customWidth="1"/>
-    <col min="7" max="7" width="24.6328125" customWidth="1"/>
-    <col min="8" max="8" width="27.6328125" customWidth="1"/>
-    <col min="9" max="9" width="13.08984375" customWidth="1"/>
-    <col min="10" max="11" width="8.6328125" customWidth="1"/>
-    <col min="12" max="12" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="8.6328125" customWidth="1"/>
-    <col min="16" max="16" width="200.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.44140625" customWidth="1"/>
+    <col min="4" max="4" width="35.44140625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="23.109375" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" customWidth="1"/>
+    <col min="7" max="7" width="24.6640625" customWidth="1"/>
+    <col min="8" max="8" width="27.6640625" customWidth="1"/>
+    <col min="9" max="9" width="13.109375" customWidth="1"/>
+    <col min="10" max="11" width="8.6640625" customWidth="1"/>
+    <col min="12" max="12" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="8.6640625" customWidth="1"/>
+    <col min="16" max="16" width="200.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="C1" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -1633,7 +1603,7 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="G1" t="s">
         <v>3</v>
@@ -1663,13 +1633,13 @@
         <v>4</v>
       </c>
       <c r="P1" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="Q1" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="H2" t="s">
         <v>5</v>
       </c>
@@ -1695,15 +1665,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C3" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="D3" t="s">
         <v>13</v>
@@ -1712,30 +1682,30 @@
         <v>14</v>
       </c>
       <c r="F3" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="G3" t="s">
         <v>13</v>
       </c>
       <c r="H3" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="I3" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>15</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C4" t="s">
         <v>20</v>
@@ -1747,7 +1717,7 @@
         <v>22</v>
       </c>
       <c r="F4" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="G4" t="s">
         <v>21</v>
@@ -1759,79 +1729,79 @@
         <v>24</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C5" t="s">
         <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="E5" t="s">
         <v>26</v>
       </c>
       <c r="F5" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="G5" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="H5" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C6" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="D6" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="E6" t="s">
         <v>26</v>
       </c>
       <c r="F6" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="G6" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="H6" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C7" t="s">
         <v>16</v>
@@ -1843,7 +1813,7 @@
         <v>18</v>
       </c>
       <c r="F7" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="G7" t="s">
         <v>17</v>
@@ -1852,56 +1822,56 @@
         <v>19</v>
       </c>
       <c r="I7" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.35">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>1</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>32</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>29</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="P8" s="3" t="s">
         <v>33</v>
       </c>
       <c r="Q8" s="3" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C9" t="s">
         <v>34</v>
@@ -1913,7 +1883,7 @@
         <v>29</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="G9" t="s">
         <v>35</v>
@@ -1922,21 +1892,21 @@
         <v>36</v>
       </c>
       <c r="I9" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="P9" s="1" t="s">
         <v>37</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C10" t="s">
         <v>27</v>
@@ -1948,254 +1918,254 @@
         <v>29</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="G10" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="H10" t="s">
         <v>30</v>
       </c>
       <c r="I10" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="P10" s="1" t="s">
         <v>31</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C11" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D11" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E11" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="G11" t="s">
         <v>50</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="G11" t="s">
-        <v>54</v>
-      </c>
       <c r="H11" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.35">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>2</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="P12" s="3" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="Q12" s="3" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.35">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>2</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="P13" s="3" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="Q13" s="3" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="G14" t="s">
+        <v>45</v>
+      </c>
+      <c r="H14" t="s">
+        <v>47</v>
+      </c>
+      <c r="P14" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D14" t="s">
-        <v>49</v>
-      </c>
-      <c r="E14" t="s">
-        <v>50</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="G14" t="s">
-        <v>49</v>
-      </c>
-      <c r="H14" t="s">
-        <v>51</v>
-      </c>
-      <c r="P14" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="Q14" s="1" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C15" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D15" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E15" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="G15" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="H15" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.35">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>1</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="P16" s="3" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="Q16" s="3" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.35">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>1</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="P17" s="3" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="Q17" s="3" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C18" t="s">
         <v>38</v>
@@ -2207,7 +2177,7 @@
         <v>40</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="G18" t="s">
         <v>39</v>
@@ -2219,440 +2189,440 @@
         <v>42</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>1</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C19" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="D19" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="E19" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="G19" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="H19" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="P19" s="1" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>1</v>
       </c>
-      <c r="B20" t="s">
-        <v>163</v>
+      <c r="B20" s="2" t="s">
+        <v>155</v>
       </c>
       <c r="C20" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="D20" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="E20" t="s">
-        <v>45</v>
+        <v>7</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="G20" t="s">
-        <v>44</v>
-      </c>
-      <c r="H20" t="s">
-        <v>46</v>
+        <v>214</v>
+      </c>
+      <c r="J20" t="s">
+        <v>214</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>47</v>
+        <v>215</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>1</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C21" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D21" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E21" t="s">
         <v>7</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="G21" t="s">
-        <v>224</v>
+        <v>61</v>
       </c>
       <c r="J21" t="s">
-        <v>224</v>
+        <v>61</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>225</v>
+        <v>62</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>1</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C22" t="s">
+        <v>63</v>
+      </c>
+      <c r="D22" t="s">
         <v>64</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
+        <v>8</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="G22" t="s">
+        <v>64</v>
+      </c>
+      <c r="K22" t="s">
+        <v>64</v>
+      </c>
+      <c r="P22" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E22" t="s">
-        <v>7</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="G22" t="s">
+      <c r="Q22" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="J22" t="s">
-        <v>65</v>
-      </c>
-      <c r="P22" s="1" t="s">
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>4</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C23" t="s">
         <v>66</v>
       </c>
-      <c r="Q22" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A23">
-        <v>1</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>67</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>68</v>
       </c>
-      <c r="E23" t="s">
-        <v>8</v>
-      </c>
       <c r="F23" s="2" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="G23" t="s">
-        <v>68</v>
-      </c>
-      <c r="K23" t="s">
-        <v>68</v>
+        <v>67</v>
+      </c>
+      <c r="H23" t="s">
+        <v>69</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>69</v>
+        <v>172</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A24">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="2">
         <v>4</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="C24" t="s">
-        <v>70</v>
-      </c>
-      <c r="D24" t="s">
+        <v>155</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="P24" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="Q24" s="3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>6</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C25" t="s">
         <v>71</v>
       </c>
-      <c r="E24" t="s">
+      <c r="D25" t="s">
         <v>72</v>
       </c>
-      <c r="F24" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="G24" t="s">
-        <v>71</v>
-      </c>
-      <c r="H24" t="s">
+      <c r="E25" t="s">
         <v>73</v>
       </c>
-      <c r="P24" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="Q24" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="2">
-        <v>4</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>158</v>
-      </c>
       <c r="F25" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="P25" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="Q25" s="3" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
+        <v>208</v>
+      </c>
+      <c r="G25" t="s">
+        <v>72</v>
+      </c>
+      <c r="L25" t="s">
+        <v>72</v>
+      </c>
+      <c r="P25" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="Q25" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C26" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D26" t="s">
+        <v>80</v>
+      </c>
+      <c r="E26" t="s">
         <v>76</v>
       </c>
-      <c r="E26" t="s">
-        <v>77</v>
-      </c>
       <c r="F26" s="2" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
       <c r="G26" t="s">
-        <v>76</v>
-      </c>
-      <c r="L26" t="s">
-        <v>76</v>
+        <v>80</v>
+      </c>
+      <c r="H26" t="s">
+        <v>81</v>
+      </c>
+      <c r="I26" t="s">
+        <v>193</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>236</v>
+        <v>173</v>
       </c>
       <c r="Q26" s="1" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>2</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C27" t="s">
+        <v>74</v>
+      </c>
+      <c r="D27" t="s">
+        <v>75</v>
+      </c>
+      <c r="E27" t="s">
+        <v>76</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="G27" t="s">
+        <v>75</v>
+      </c>
+      <c r="H27" t="s">
+        <v>77</v>
+      </c>
+      <c r="I27" t="s">
+        <v>194</v>
+      </c>
+      <c r="P27" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q27" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C28" t="s">
         <v>83</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D28" t="s">
         <v>84</v>
       </c>
-      <c r="E27" t="s">
-        <v>80</v>
-      </c>
-      <c r="F27" s="2" t="s">
+      <c r="E28" t="s">
+        <v>85</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="G28" t="s">
+        <v>84</v>
+      </c>
+      <c r="K28" t="s">
+        <v>84</v>
+      </c>
+      <c r="P28" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q28" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="2">
+        <v>4</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="I29" t="s">
+        <v>195</v>
+      </c>
+      <c r="P29" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="G27" t="s">
-        <v>84</v>
-      </c>
-      <c r="H27" t="s">
-        <v>85</v>
-      </c>
-      <c r="I27" t="s">
-        <v>203</v>
-      </c>
-      <c r="P27" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="Q27" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A28">
-        <v>2</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="C28" t="s">
-        <v>78</v>
-      </c>
-      <c r="D28" t="s">
-        <v>79</v>
-      </c>
-      <c r="E28" t="s">
-        <v>80</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="G28" t="s">
-        <v>79</v>
-      </c>
-      <c r="H28" t="s">
-        <v>81</v>
-      </c>
-      <c r="I28" t="s">
-        <v>204</v>
-      </c>
-      <c r="P28" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="Q28" s="1" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A29">
+      <c r="Q29" s="3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>4</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C30" t="s">
+        <v>88</v>
+      </c>
+      <c r="D30" s="4">
+        <v>4708</v>
+      </c>
+      <c r="E30" t="s">
+        <v>200</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="G30" s="4">
+        <v>4708</v>
+      </c>
+      <c r="H30" t="s">
+        <v>199</v>
+      </c>
+      <c r="P30" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="Q30" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A31">
         <v>1</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="C29" t="s">
-        <v>87</v>
-      </c>
-      <c r="D29" t="s">
-        <v>88</v>
-      </c>
-      <c r="E29" t="s">
+      <c r="B31" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C31" t="s">
         <v>89</v>
       </c>
-      <c r="F29" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="G29" t="s">
-        <v>88</v>
-      </c>
-      <c r="K29" t="s">
-        <v>88</v>
-      </c>
-      <c r="P29" s="1" t="s">
+      <c r="D31" t="s">
         <v>90</v>
       </c>
-      <c r="Q29" s="1" t="s">
+      <c r="E31" t="s">
+        <v>91</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="G31" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="30" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="2">
-        <v>4</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="I30" t="s">
-        <v>205</v>
-      </c>
-      <c r="P30" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="Q30" s="3" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A31">
-        <v>4</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="C31" t="s">
+      <c r="M31" t="s">
+        <v>90</v>
+      </c>
+      <c r="P31" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D31" s="4">
-        <v>4708</v>
-      </c>
-      <c r="E31" t="s">
-        <v>210</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="G31" s="4">
-        <v>4708</v>
-      </c>
-      <c r="H31" t="s">
-        <v>209</v>
-      </c>
-      <c r="P31" s="1" t="s">
-        <v>211</v>
-      </c>
       <c r="Q31" s="1" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>1</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C32" t="s">
         <v>93</v>
@@ -2664,285 +2634,229 @@
         <v>95</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="G32" t="s">
         <v>94</v>
       </c>
-      <c r="M32" t="s">
-        <v>94</v>
+      <c r="H32" t="s">
+        <v>96</v>
+      </c>
+      <c r="I32" t="s">
+        <v>196</v>
       </c>
       <c r="P32" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="Q32" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.35">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>1</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C33" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D33" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E33" t="s">
+        <v>100</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="G33" t="s">
         <v>99</v>
       </c>
-      <c r="F33" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="G33" t="s">
-        <v>98</v>
-      </c>
-      <c r="H33" t="s">
-        <v>100</v>
-      </c>
-      <c r="I33" t="s">
-        <v>206</v>
+      <c r="N33" t="s">
+        <v>101</v>
       </c>
       <c r="P33" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="Q33" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.35">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>1</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C34" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
       <c r="D34" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
       <c r="E34" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="G34" t="s">
-        <v>103</v>
-      </c>
-      <c r="N34" t="s">
-        <v>105</v>
+        <v>114</v>
+      </c>
+      <c r="O34" t="s">
+        <v>114</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>106</v>
+        <v>198</v>
       </c>
       <c r="Q34" s="1" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.35">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>1</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C35" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="D35" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="E35" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="G35" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="O35" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="P35" s="1" t="s">
-        <v>208</v>
+        <v>223</v>
       </c>
       <c r="Q35" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.35">
+        <v>174</v>
+      </c>
+      <c r="R35" t="s">
+        <v>224</v>
+      </c>
+      <c r="S35" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>1</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C36" t="s">
+        <v>106</v>
+      </c>
+      <c r="D36" t="s">
+        <v>106</v>
+      </c>
+      <c r="E36" t="s">
         <v>107</v>
       </c>
-      <c r="D36" t="s">
+      <c r="F36" t="s">
+        <v>208</v>
+      </c>
+      <c r="G36" t="s">
+        <v>106</v>
+      </c>
+      <c r="O36" t="s">
         <v>108</v>
       </c>
-      <c r="E36" t="s">
-        <v>109</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="G36" t="s">
-        <v>108</v>
-      </c>
-      <c r="O36" t="s">
-        <v>107</v>
-      </c>
       <c r="P36" s="1" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
       <c r="Q36" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="R36" t="s">
-        <v>234</v>
-      </c>
-      <c r="S36" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="37" spans="1:19" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>1</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C37" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D37" t="s">
-        <v>110</v>
+        <v>204</v>
       </c>
       <c r="E37" t="s">
-        <v>111</v>
+        <v>203</v>
       </c>
       <c r="F37" t="s">
+        <v>213</v>
+      </c>
+      <c r="G37" t="s">
+        <v>220</v>
+      </c>
+      <c r="I37" t="s">
+        <v>219</v>
+      </c>
+      <c r="P37" t="s">
         <v>218</v>
       </c>
-      <c r="G37" t="s">
-        <v>110</v>
-      </c>
-      <c r="O37" t="s">
-        <v>112</v>
-      </c>
-      <c r="P37" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="Q37" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="Q37" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>1</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>164</v>
+      <c r="B38" t="s">
+        <v>154</v>
       </c>
       <c r="C38" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D38" t="s">
-        <v>214</v>
+        <v>111</v>
       </c>
       <c r="E38" t="s">
-        <v>213</v>
+        <v>112</v>
       </c>
       <c r="F38" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="G38" t="s">
-        <v>230</v>
-      </c>
-      <c r="I38" t="s">
-        <v>229</v>
-      </c>
-      <c r="P38" t="s">
-        <v>228</v>
-      </c>
-      <c r="Q38" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A39">
-        <v>10</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="C39" t="s">
-        <v>120</v>
-      </c>
-      <c r="D39" t="s">
-        <v>121</v>
-      </c>
-      <c r="E39" t="s">
-        <v>122</v>
-      </c>
-      <c r="F39" t="s">
-        <v>218</v>
-      </c>
-      <c r="G39" t="s">
-        <v>121</v>
-      </c>
-      <c r="N39" t="s">
-        <v>123</v>
-      </c>
-      <c r="P39" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="Q39" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A40">
-        <v>1</v>
-      </c>
-      <c r="B40" t="s">
-        <v>163</v>
-      </c>
-      <c r="C40" t="s">
-        <v>114</v>
-      </c>
-      <c r="D40" t="s">
-        <v>115</v>
-      </c>
-      <c r="E40" t="s">
-        <v>116</v>
-      </c>
-      <c r="F40" t="s">
-        <v>218</v>
-      </c>
-      <c r="G40" t="s">
-        <v>115</v>
-      </c>
-      <c r="O40" t="s">
-        <v>114</v>
-      </c>
-      <c r="P40" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="Q40" s="1" t="s">
-        <v>185</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="O38" t="s">
+        <v>110</v>
+      </c>
+      <c r="P38" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="Q38" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="Q39" s="1"/>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="F40" s="2"/>
+      <c r="P40" s="1"/>
+      <c r="Q40" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2954,68 +2868,64 @@
     <hyperlink ref="P8" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
     <hyperlink ref="P9" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
     <hyperlink ref="P18" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="P20" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="P14" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="P12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="P11" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="P15" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="P16" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="P17" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="P22" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="P23" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="P24" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="P25" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="P28" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="P27" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="P29" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="P31" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="P32" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="P33" r:id="rId25" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="P34" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="P40" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="P39" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="P3" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="P4" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="P13" r:id="rId31" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="Q3" r:id="rId32" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="Q4" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="Q5" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="Q6" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="Q7" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="Q8" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="Q9" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="Q10" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="Q11" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="Q12" r:id="rId41" display="https://www.digikey.ca/product-detail/en/molex-connector-corporation/22-05-2031/WM4101-ND/" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="Q13" r:id="rId42" display="https://www.digikey.ca/product-detail/en/preci-dip/801-87-003-10-001101/1212-1180-ND" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="Q14" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="Q15" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="Q16" r:id="rId45" display="https://www.digikey.ca/product-detail/en/everlight-electronics-co-ltd/MV5437/1080-1109-ND/2675600" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="Q17" r:id="rId46" display="https://www.digikey.ca/product-detail/en/sullins-connector-solutions/SPC02SYAN/S9002-ND" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="Q18" r:id="rId47" display="http://www.digikey.ca/product-detail/en/fairchild-on-semiconductor/2N3906TFR/2N3906D26ZCT-ND" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink ref="Q19" r:id="rId48" display="https://www.digikey.ca/product-detail/en/sullins-connector-solutions/PPPC061LFBN-RC/S7039-ND" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="Q20" r:id="rId49" display="http://www.digikey.ca/product-detail/en/3m/929974-01-01/929974-01-01-ND" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="Q22" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink ref="Q23" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="Q24" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="Q25" r:id="rId53" display="https://www.digikey.ca/product-detail/en/essentra-components/NMS-308/RP809-ND" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink ref="Q27" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink ref="Q28" r:id="rId55" display="http://www.digikey.ca/product-detail/en/keystone-electronics/25503/36-25503-ND/" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink ref="Q29" r:id="rId56" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
-    <hyperlink ref="Q30" r:id="rId57" display="https://www.digikey.ca/product-detail/en/3m/SJ-5003-(BLACK)/SJ5003-0-ND/102573" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink ref="Q31" r:id="rId58" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="Q32" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
-    <hyperlink ref="Q33" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
-    <hyperlink ref="Q35" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
-    <hyperlink ref="Q36" r:id="rId62" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
-    <hyperlink ref="Q37" r:id="rId63" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink ref="Q39" r:id="rId64" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
-    <hyperlink ref="Q40" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
-    <hyperlink ref="P35" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
-    <hyperlink ref="P36" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
-    <hyperlink ref="Q34" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
-    <hyperlink ref="P26" r:id="rId69" xr:uid="{4CCDA3FE-08D0-46DF-9B30-73A601C4D5A0}"/>
-    <hyperlink ref="Q26" r:id="rId70" xr:uid="{4DAFF11F-FB4D-4481-B87D-4D729F143D51}"/>
+    <hyperlink ref="P14" r:id="rId9" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="P12" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="P11" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="P15" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="P16" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="P17" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="P21" r:id="rId15" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="P22" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="P23" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="P24" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="P27" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="P26" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="P28" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="P30" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="P31" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="P32" r:id="rId24" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="P33" r:id="rId25" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="P38" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="P3" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="P4" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="P13" r:id="rId29" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="Q3" r:id="rId30" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="Q4" r:id="rId31" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="Q5" r:id="rId32" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="Q6" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="Q7" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="Q8" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="Q9" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="Q10" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="Q11" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="Q12" r:id="rId39" display="https://www.digikey.ca/product-detail/en/molex-connector-corporation/22-05-2031/WM4101-ND/" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="Q13" r:id="rId40" display="https://www.digikey.ca/product-detail/en/preci-dip/801-87-003-10-001101/1212-1180-ND" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="Q14" r:id="rId41" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="Q15" r:id="rId42" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="Q16" r:id="rId43" display="https://www.digikey.ca/product-detail/en/everlight-electronics-co-ltd/MV5437/1080-1109-ND/2675600" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="Q17" r:id="rId44" display="https://www.digikey.ca/product-detail/en/sullins-connector-solutions/SPC02SYAN/S9002-ND" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="Q18" r:id="rId45" display="http://www.digikey.ca/product-detail/en/fairchild-on-semiconductor/2N3906TFR/2N3906D26ZCT-ND" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="Q19" r:id="rId46" display="https://www.digikey.ca/product-detail/en/sullins-connector-solutions/PPPC061LFBN-RC/S7039-ND" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="Q21" r:id="rId47" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="Q22" r:id="rId48" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="Q23" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="Q24" r:id="rId50" display="https://www.digikey.ca/product-detail/en/essentra-components/NMS-308/RP809-ND" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="Q26" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="Q27" r:id="rId52" display="http://www.digikey.ca/product-detail/en/keystone-electronics/25503/36-25503-ND/" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="Q28" r:id="rId53" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="Q29" r:id="rId54" display="https://www.digikey.ca/product-detail/en/3m/SJ-5003-(BLACK)/SJ5003-0-ND/102573" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="Q30" r:id="rId55" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="Q31" r:id="rId56" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="Q32" r:id="rId57" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="Q34" r:id="rId58" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="Q35" r:id="rId59" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="Q36" r:id="rId60" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="Q38" r:id="rId61" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="P34" r:id="rId62" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="P35" r:id="rId63" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="Q33" r:id="rId64" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="P25" r:id="rId65" xr:uid="{4CCDA3FE-08D0-46DF-9B30-73A601C4D5A0}"/>
+    <hyperlink ref="Q25" r:id="rId66" xr:uid="{4DAFF11F-FB4D-4481-B87D-4D729F143D51}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>